<commit_message>
Merging with the home code
Added all the routes and the changes with it
</commit_message>
<xml_diff>
--- a/Scripts/sql/units_metaData.xlsx
+++ b/Scripts/sql/units_metaData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9BAF0773-1809-4F55-8F78-9CEF8502C683}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="161">
   <si>
     <t>UNIT_RACE</t>
   </si>
@@ -497,223 +498,13 @@
     <t>UNIT_ICON</t>
   </si>
   <si>
-    <t>UNIT_IMAGE</t>
-  </si>
-  <si>
-    <t>r01.png</t>
-  </si>
-  <si>
-    <t>r02.png</t>
-  </si>
-  <si>
-    <t>r03.png</t>
-  </si>
-  <si>
-    <t>r04.png</t>
-  </si>
-  <si>
-    <t>r05.png</t>
-  </si>
-  <si>
-    <t>r06.png</t>
-  </si>
-  <si>
-    <t>r07.png</t>
-  </si>
-  <si>
-    <t>r08.png</t>
-  </si>
-  <si>
-    <t>r09.png</t>
-  </si>
-  <si>
-    <t>r10.png</t>
-  </si>
-  <si>
-    <t>t01.png</t>
-  </si>
-  <si>
-    <t>t02.png</t>
-  </si>
-  <si>
-    <t>t03.png</t>
-  </si>
-  <si>
-    <t>t04.png</t>
-  </si>
-  <si>
-    <t>t05.png</t>
-  </si>
-  <si>
-    <t>t06.png</t>
-  </si>
-  <si>
-    <t>t07.png</t>
-  </si>
-  <si>
-    <t>t08.png</t>
-  </si>
-  <si>
-    <t>t09.png</t>
-  </si>
-  <si>
-    <t>t10.png</t>
-  </si>
-  <si>
-    <t>g01.png</t>
-  </si>
-  <si>
-    <t>g02.png</t>
-  </si>
-  <si>
-    <t>g03.png</t>
-  </si>
-  <si>
-    <t>g04.png</t>
-  </si>
-  <si>
-    <t>g05.png</t>
-  </si>
-  <si>
-    <t>g06.png</t>
-  </si>
-  <si>
-    <t>g07.png</t>
-  </si>
-  <si>
-    <t>g08.png</t>
-  </si>
-  <si>
-    <t>g09.png</t>
-  </si>
-  <si>
-    <t>g10.png</t>
-  </si>
-  <si>
-    <t>a01.png</t>
-  </si>
-  <si>
-    <t>a02.png</t>
-  </si>
-  <si>
-    <t>a03.png</t>
-  </si>
-  <si>
-    <t>a04.png</t>
-  </si>
-  <si>
-    <t>a05.png</t>
-  </si>
-  <si>
-    <t>a06.png</t>
-  </si>
-  <si>
-    <t>a07.png</t>
-  </si>
-  <si>
-    <t>a08.png</t>
-  </si>
-  <si>
-    <t>a09.png</t>
-  </si>
-  <si>
-    <t>a10.png</t>
-  </si>
-  <si>
-    <t>n01.png</t>
-  </si>
-  <si>
-    <t>n02.png</t>
-  </si>
-  <si>
-    <t>n03.png</t>
-  </si>
-  <si>
-    <t>n04.png</t>
-  </si>
-  <si>
-    <t>n05.png</t>
-  </si>
-  <si>
-    <t>n06.png</t>
-  </si>
-  <si>
-    <t>n07.png</t>
-  </si>
-  <si>
-    <t>n08.png</t>
-  </si>
-  <si>
-    <t>n09.png</t>
-  </si>
-  <si>
-    <t>n10.png</t>
-  </si>
-  <si>
-    <t>e01.png</t>
-  </si>
-  <si>
-    <t>e02.png</t>
-  </si>
-  <si>
-    <t>e03.png</t>
-  </si>
-  <si>
-    <t>e04.png</t>
-  </si>
-  <si>
-    <t>e05.png</t>
-  </si>
-  <si>
-    <t>e06.png</t>
-  </si>
-  <si>
-    <t>e07.png</t>
-  </si>
-  <si>
-    <t>e08.png</t>
-  </si>
-  <si>
-    <t>e09.png</t>
-  </si>
-  <si>
-    <t>e10.png</t>
-  </si>
-  <si>
-    <t>h01.png</t>
-  </si>
-  <si>
-    <t>h02.png</t>
-  </si>
-  <si>
-    <t>h03.png</t>
-  </si>
-  <si>
-    <t>h04.png</t>
-  </si>
-  <si>
-    <t>h05.png</t>
-  </si>
-  <si>
-    <t>h06.png</t>
-  </si>
-  <si>
-    <t>h07.png</t>
-  </si>
-  <si>
-    <t>h08.png</t>
-  </si>
-  <si>
-    <t>h09.png</t>
-  </si>
-  <si>
-    <t>h10.png</t>
+    <t>Array String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -848,7 +639,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -856,6 +647,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -904,7 +698,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -937,9 +731,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -972,6 +783,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1147,13 +975,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2:V71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,8 +1000,10 @@
     <col min="17" max="17" width="10.6640625" customWidth="1"/>
     <col min="18" max="18" width="10.44140625" customWidth="1"/>
     <col min="19" max="19" width="9.77734375" customWidth="1"/>
-    <col min="20" max="22" width="11.109375" customWidth="1"/>
+    <col min="20" max="21" width="11.109375" customWidth="1"/>
+    <col min="22" max="22" width="77.6640625" customWidth="1"/>
     <col min="23" max="23" width="49.44140625" customWidth="1"/>
+    <col min="24" max="24" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1240,7 +1070,7 @@
       <c r="U1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>160</v>
       </c>
       <c r="W1" s="2" t="s">
@@ -1308,12 +1138,17 @@
       <c r="T2" s="3">
         <v>0</v>
       </c>
-      <c r="U2" t="s">
-        <v>161</v>
+      <c r="U2" t="str">
+        <f>A2</f>
+        <v>r01</v>
+      </c>
+      <c r="V2" t="str">
+        <f>CONCATENATE("array('id'=&gt;'",A2,"','tribe'=&gt;'",B2,"','tribe_id'=&gt;'",C2,"','name'=&gt;'",D2,"','type'=&gt;'",E2,"','upkeep'=&gt;'",F2,"','carry'=&gt;'",G2,"','speed'=&gt;'",H2,"','offense'=&gt;'",I2,"','offense_max'=&gt;'",J2,"','defense_inf'=&gt;'",K2,"','defense_inf_max'=&gt;'",L2,"','defense_cav'=&gt;'",M2,"','defense_cav_max'=&gt;'",N2,"','cost'=&gt;'",O2,"','cost_wood'=&gt;'",P2,"','cost_clay'=&gt;'",Q2,"','cost_iron'=&gt;'",R2,"','cost_crop'=&gt;'",S2,"','time'=&gt;'",T2,"','image'=&gt;'",U2,"'),")</f>
+        <v>array('id'=&gt;'r01','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Legionnaire','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'6','offense'=&gt;'40','offense_max'=&gt;'52.4','defense_inf'=&gt;'35','defense_inf_max'=&gt;'46.6','defense_cav'=&gt;'50','defense_cav_max'=&gt;'63.9','cost'=&gt;'400','cost_wood'=&gt;'120','cost_clay'=&gt;'100','cost_iron'=&gt;'150','cost_crop'=&gt;'30','time'=&gt;'0','image'=&gt;'r01'),</v>
       </c>
       <c r="W2" t="str">
         <f>CONCATENATE("INSERT INTO UNITS_DETAILS VALUES ('",A2,"','",B2,"',",C2,",'",D2,"',",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2,",",M2,",",N2,",",O2,",",P2,",",Q2,",",R2,",",S2,",",T2,",'",U2,"','",V2,"');")</f>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r01','Roman',1,'Legionnaire',3,1,50,6,40,52.4,35,46.6,50,63.9,400,120,100,150,30,0,'r01.png','');</v>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r01','Roman',1,'Legionnaire',3,1,50,6,40,52.4,35,46.6,50,63.9,400,120,100,150,30,0,'r01','array('id'=&gt;'r01','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Legionnaire','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'6','offense'=&gt;'40','offense_max'=&gt;'52.4','defense_inf'=&gt;'35','defense_inf_max'=&gt;'46.6','defense_cav'=&gt;'50','defense_cav_max'=&gt;'63.9','cost'=&gt;'400','cost_wood'=&gt;'120','cost_clay'=&gt;'100','cost_iron'=&gt;'150','cost_crop'=&gt;'30','time'=&gt;'0','image'=&gt;'r01'),');</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -1377,12 +1212,17 @@
       <c r="T3" s="3">
         <v>0</v>
       </c>
-      <c r="U3" t="s">
-        <v>162</v>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U66" si="0">A3</f>
+        <v>r02</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V66" si="1">CONCATENATE("array('id'=&gt;'",A3,"','tribe'=&gt;'",B3,"','tribe_id'=&gt;'",C3,"','name'=&gt;'",D3,"','type'=&gt;'",E3,"','upkeep'=&gt;'",F3,"','carry'=&gt;'",G3,"','speed'=&gt;'",H3,"','offense'=&gt;'",I3,"','offense_max'=&gt;'",J3,"','defense_inf'=&gt;'",K3,"','defense_inf_max'=&gt;'",L3,"','defense_cav'=&gt;'",M3,"','defense_cav_max'=&gt;'",N3,"','cost'=&gt;'",O3,"','cost_wood'=&gt;'",P3,"','cost_clay'=&gt;'",Q3,"','cost_iron'=&gt;'",R3,"','cost_crop'=&gt;'",S3,"','time'=&gt;'",T3,"','image'=&gt;'",U3,"'),")</f>
+        <v>array('id'=&gt;'r02','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Praetorian','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'20','speed'=&gt;'5','offense'=&gt;'30','offense_max'=&gt;'40.9','defense_inf'=&gt;'65','defense_inf_max'=&gt;'81.1','defense_cav'=&gt;'35','defense_cav_max'=&gt;'46.6','cost'=&gt;'460','cost_wood'=&gt;'100','cost_clay'=&gt;'130','cost_iron'=&gt;'160','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'r02'),</v>
       </c>
       <c r="W3" t="str">
-        <f t="shared" ref="W3:W66" si="0">CONCATENATE("INSERT INTO UNITS_DETAILS VALUES ('",A3,"','",B3,"',",C3,",'",D3,"',",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3,",",M3,",",N3,",",O3,",",P3,",",Q3,",",R3,",",S3,",",T3,",'",U3,"','",V3,"');")</f>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r02','Roman',1,'Praetorian',1,1,20,5,30,40.9,65,81.1,35,46.6,460,100,130,160,70,0,'r02.png','');</v>
+        <f t="shared" ref="W3:W66" si="2">CONCATENATE("INSERT INTO UNITS_DETAILS VALUES ('",A3,"','",B3,"',",C3,",'",D3,"',",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3,",",M3,",",N3,",",O3,",",P3,",",Q3,",",R3,",",S3,",",T3,",'",U3,"','",V3,"');")</f>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r02','Roman',1,'Praetorian',1,1,20,5,30,40.9,65,81.1,35,46.6,460,100,130,160,70,0,'r02','array('id'=&gt;'r02','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Praetorian','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'20','speed'=&gt;'5','offense'=&gt;'30','offense_max'=&gt;'40.9','defense_inf'=&gt;'65','defense_inf_max'=&gt;'81.1','defense_cav'=&gt;'35','defense_cav_max'=&gt;'46.6','cost'=&gt;'460','cost_wood'=&gt;'100','cost_clay'=&gt;'130','cost_iron'=&gt;'160','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'r02'),');</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -1446,12 +1286,17 @@
       <c r="T4" s="3">
         <v>0</v>
       </c>
-      <c r="U4" t="s">
-        <v>163</v>
+      <c r="U4" t="str">
+        <f t="shared" si="0"/>
+        <v>r03</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r03','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Imperian','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'7','offense'=&gt;'70','offense_max'=&gt;'86.9','defense_inf'=&gt;'40','defense_inf_max'=&gt;'52.4','defense_cav'=&gt;'25','defense_cav_max'=&gt;'35.1','cost'=&gt;'600','cost_wood'=&gt;'150','cost_clay'=&gt;'160','cost_iron'=&gt;'210','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'r03'),</v>
       </c>
       <c r="W4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r03','Roman',1,'Imperian',2,1,50,7,70,86.9,40,52.4,25,35.1,600,150,160,210,80,0,'r03.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r03','Roman',1,'Imperian',2,1,50,7,70,86.9,40,52.4,25,35.1,600,150,160,210,80,0,'r03','array('id'=&gt;'r03','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Imperian','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'7','offense'=&gt;'70','offense_max'=&gt;'86.9','defense_inf'=&gt;'40','defense_inf_max'=&gt;'52.4','defense_cav'=&gt;'25','defense_cav_max'=&gt;'35.1','cost'=&gt;'600','cost_wood'=&gt;'150','cost_clay'=&gt;'160','cost_iron'=&gt;'210','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'r03'),');</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
@@ -1515,12 +1360,17 @@
       <c r="T5" s="3">
         <v>0</v>
       </c>
-      <c r="U5" t="s">
-        <v>164</v>
+      <c r="U5" t="str">
+        <f t="shared" si="0"/>
+        <v>r04</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r04','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Equites Legati','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'16','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'360','cost_wood'=&gt;'140','cost_clay'=&gt;'160','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'r04'),</v>
       </c>
       <c r="W5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r04','Roman',1,'Equites Legati',0,2,0,16,0,12.7,20,35.7,10,24.2,360,140,160,20,40,0,'r04.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r04','Roman',1,'Equites Legati',0,2,0,16,0,12.7,20,35.7,10,24.2,360,140,160,20,40,0,'r04','array('id'=&gt;'r04','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Equites Legati','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'16','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'360','cost_wood'=&gt;'140','cost_clay'=&gt;'160','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'r04'),');</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -1584,12 +1434,17 @@
       <c r="T6" s="3">
         <v>0</v>
       </c>
-      <c r="U6" t="s">
-        <v>165</v>
+      <c r="U6" t="str">
+        <f t="shared" si="0"/>
+        <v>r05</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r05','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Equites Imperatoris','type'=&gt;'4','upkeep'=&gt;'3','carry'=&gt;'100','speed'=&gt;'14','offense'=&gt;'120','offense_max'=&gt;'157.1','defense_inf'=&gt;'65','defense_inf_max'=&gt;'93.9','defense_cav'=&gt;'50','defense_cav_max'=&gt;'76.6','cost'=&gt;'1410','cost_wood'=&gt;'550','cost_clay'=&gt;'440','cost_iron'=&gt;'320','cost_crop'=&gt;'100','time'=&gt;'0','image'=&gt;'r05'),</v>
       </c>
       <c r="W6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r05','Roman',1,'Equites Imperatoris',4,3,100,14,120,157.1,65,93.9,50,76.6,1410,550,440,320,100,0,'r05.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r05','Roman',1,'Equites Imperatoris',4,3,100,14,120,157.1,65,93.9,50,76.6,1410,550,440,320,100,0,'r05','array('id'=&gt;'r05','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Equites Imperatoris','type'=&gt;'4','upkeep'=&gt;'3','carry'=&gt;'100','speed'=&gt;'14','offense'=&gt;'120','offense_max'=&gt;'157.1','defense_inf'=&gt;'65','defense_inf_max'=&gt;'93.9','defense_cav'=&gt;'50','defense_cav_max'=&gt;'76.6','cost'=&gt;'1410','cost_wood'=&gt;'550','cost_clay'=&gt;'440','cost_iron'=&gt;'320','cost_crop'=&gt;'100','time'=&gt;'0','image'=&gt;'r05'),');</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -1653,12 +1508,17 @@
       <c r="T7" s="3">
         <v>0</v>
       </c>
-      <c r="U7" t="s">
-        <v>166</v>
+      <c r="U7" t="str">
+        <f t="shared" si="0"/>
+        <v>r06</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r06','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Equites Caesaris','type'=&gt;'7','upkeep'=&gt;'4','carry'=&gt;'70','speed'=&gt;'10','offense'=&gt;'180','offense_max'=&gt;'232.4','defense_inf'=&gt;'80','defense_inf_max'=&gt;'117.5','defense_cav'=&gt;'105','defense_cav_max'=&gt;'146.2','cost'=&gt;'2170','cost_wood'=&gt;'550','cost_clay'=&gt;'640','cost_iron'=&gt;'800','cost_crop'=&gt;'180','time'=&gt;'0','image'=&gt;'r06'),</v>
       </c>
       <c r="W7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r06','Roman',1,'Equites Caesaris',7,4,70,10,180,232.4,80,117.5,105,146.2,2170,550,640,800,180,0,'r06.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r06','Roman',1,'Equites Caesaris',7,4,70,10,180,232.4,80,117.5,105,146.2,2170,550,640,800,180,0,'r06','array('id'=&gt;'r06','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Equites Caesaris','type'=&gt;'7','upkeep'=&gt;'4','carry'=&gt;'70','speed'=&gt;'10','offense'=&gt;'180','offense_max'=&gt;'232.4','defense_inf'=&gt;'80','defense_inf_max'=&gt;'117.5','defense_cav'=&gt;'105','defense_cav_max'=&gt;'146.2','cost'=&gt;'2170','cost_wood'=&gt;'550','cost_clay'=&gt;'640','cost_iron'=&gt;'800','cost_crop'=&gt;'180','time'=&gt;'0','image'=&gt;'r06'),');</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -1722,12 +1582,17 @@
       <c r="T8" s="3">
         <v>0</v>
       </c>
-      <c r="U8" t="s">
-        <v>167</v>
+      <c r="U8" t="str">
+        <f t="shared" si="0"/>
+        <v>r07</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r07','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Battering Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'60','offense_max'=&gt;'88.1','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'75','defense_cav_max'=&gt;'105.3','cost'=&gt;'1830','cost_wood'=&gt;'900','cost_clay'=&gt;'360','cost_iron'=&gt;'500','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'r07'),</v>
       </c>
       <c r="W8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r07','Roman',1,'Battering Ram',6,3,0,4,60,88.1,30,53.6,75,105.3,1830,900,360,500,70,0,'r07.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r07','Roman',1,'Battering Ram',6,3,0,4,60,88.1,30,53.6,75,105.3,1830,900,360,500,70,0,'r07','array('id'=&gt;'r07','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Battering Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'60','offense_max'=&gt;'88.1','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'75','defense_cav_max'=&gt;'105.3','cost'=&gt;'1830','cost_wood'=&gt;'900','cost_clay'=&gt;'360','cost_iron'=&gt;'500','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'r07'),');</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -1791,12 +1656,17 @@
       <c r="T9" s="3">
         <v>0</v>
       </c>
-      <c r="U9" t="s">
-        <v>168</v>
+      <c r="U9" t="str">
+        <f t="shared" si="0"/>
+        <v>r08</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r08','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Fire Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'75','offense_max'=&gt;'124.5','defense_inf'=&gt;'60','defense_inf_max'=&gt;'107.2','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'2990','cost_wood'=&gt;'950','cost_clay'=&gt;'1350','cost_iron'=&gt;'600','cost_crop'=&gt;'90','time'=&gt;'0','image'=&gt;'r08'),</v>
       </c>
       <c r="W9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r08','Roman',1,'Fire Catapult',6,6,0,3,75,124.5,60,107.2,10,49.7,2990,950,1350,600,90,0,'r08.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r08','Roman',1,'Fire Catapult',6,6,0,3,75,124.5,60,107.2,10,49.7,2990,950,1350,600,90,0,'r08','array('id'=&gt;'r08','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Fire Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'75','offense_max'=&gt;'124.5','defense_inf'=&gt;'60','defense_inf_max'=&gt;'107.2','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'2990','cost_wood'=&gt;'950','cost_clay'=&gt;'1350','cost_iron'=&gt;'600','cost_crop'=&gt;'90','time'=&gt;'0','image'=&gt;'r08'),');</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
@@ -1860,12 +1730,17 @@
       <c r="T10" s="3">
         <v>0</v>
       </c>
-      <c r="U10" t="s">
-        <v>169</v>
+      <c r="U10" t="str">
+        <f t="shared" si="0"/>
+        <v>r09</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r09','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Senator','type'=&gt;'8','upkeep'=&gt;'5','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'50','offense_max'=&gt;'50','defense_inf'=&gt;'40','defense_inf_max'=&gt;'40','defense_cav'=&gt;'30','defense_cav_max'=&gt;'30','cost'=&gt;'140450','cost_wood'=&gt;'30750','cost_clay'=&gt;'27200','cost_iron'=&gt;'45000','cost_crop'=&gt;'37500','time'=&gt;'0','image'=&gt;'r09'),</v>
       </c>
       <c r="W10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r09','Roman',1,'Senator',8,5,0,4,50,50,40,40,30,30,140450,30750,27200,45000,37500,0,'r09.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r09','Roman',1,'Senator',8,5,0,4,50,50,40,40,30,30,140450,30750,27200,45000,37500,0,'r09','array('id'=&gt;'r09','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Senator','type'=&gt;'8','upkeep'=&gt;'5','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'50','offense_max'=&gt;'50','defense_inf'=&gt;'40','defense_inf_max'=&gt;'40','defense_cav'=&gt;'30','defense_cav_max'=&gt;'30','cost'=&gt;'140450','cost_wood'=&gt;'30750','cost_clay'=&gt;'27200','cost_iron'=&gt;'45000','cost_crop'=&gt;'37500','time'=&gt;'0','image'=&gt;'r09'),');</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -1929,12 +1804,17 @@
       <c r="T11" s="3">
         <v>0</v>
       </c>
-      <c r="U11" t="s">
-        <v>170</v>
+      <c r="U11" t="str">
+        <f t="shared" si="0"/>
+        <v>r10</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'r10','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'19000','cost_wood'=&gt;'4600','cost_clay'=&gt;'4200','cost_iron'=&gt;'5800','cost_crop'=&gt;'4400','time'=&gt;'0','image'=&gt;'r10'),</v>
       </c>
       <c r="W11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('r10','Roman',1,'Settler',8,1,3000,5,0,0,80,80,80,80,19000,4600,4200,5800,4400,0,'r10.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('r10','Roman',1,'Settler',8,1,3000,5,0,0,80,80,80,80,19000,4600,4200,5800,4400,0,'r10','array('id'=&gt;'r10','tribe'=&gt;'Roman','tribe_id'=&gt;'1','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'19000','cost_wood'=&gt;'4600','cost_clay'=&gt;'4200','cost_iron'=&gt;'5800','cost_crop'=&gt;'4400','time'=&gt;'0','image'=&gt;'r10'),');</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
@@ -1998,12 +1878,17 @@
       <c r="T12" s="3">
         <v>0</v>
       </c>
-      <c r="U12" t="s">
-        <v>171</v>
+      <c r="U12" t="str">
+        <f t="shared" si="0"/>
+        <v>t01</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t01','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Maceman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'60','speed'=&gt;'7','offense'=&gt;'40','offense_max'=&gt;'52.4','defense_inf'=&gt;'20','defense_inf_max'=&gt;'29.4','defense_cav'=&gt;'5','defense_cav_max'=&gt;'12.1','cost'=&gt;'250','cost_wood'=&gt;'95','cost_clay'=&gt;'75','cost_iron'=&gt;'40','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'t01'),</v>
       </c>
       <c r="W12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t01','Teuton',2,'Maceman',2,1,60,7,40,52.4,20,29.4,5,12.1,250,95,75,40,40,0,'t01.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t01','Teuton',2,'Maceman',2,1,60,7,40,52.4,20,29.4,5,12.1,250,95,75,40,40,0,'t01','array('id'=&gt;'t01','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Maceman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'60','speed'=&gt;'7','offense'=&gt;'40','offense_max'=&gt;'52.4','defense_inf'=&gt;'20','defense_inf_max'=&gt;'29.4','defense_cav'=&gt;'5','defense_cav_max'=&gt;'12.1','cost'=&gt;'250','cost_wood'=&gt;'95','cost_clay'=&gt;'75','cost_iron'=&gt;'40','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'t01'),');</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
@@ -2067,12 +1952,17 @@
       <c r="T13" s="3">
         <v>0</v>
       </c>
-      <c r="U13" t="s">
-        <v>172</v>
+      <c r="U13" t="str">
+        <f t="shared" si="0"/>
+        <v>t02</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t02','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Spearman','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'40','speed'=&gt;'7','offense'=&gt;'10','offense_max'=&gt;'17.9','defense_inf'=&gt;'35','defense_inf_max'=&gt;'46.6','defense_cav'=&gt;'60','defense_cav_max'=&gt;'75.4','cost'=&gt;'340','cost_wood'=&gt;'145','cost_clay'=&gt;'70','cost_iron'=&gt;'85','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'t02'),</v>
       </c>
       <c r="W13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t02','Teuton',2,'Spearman',1,1,40,7,10,17.9,35,46.6,60,75.4,340,145,70,85,40,0,'t02.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t02','Teuton',2,'Spearman',1,1,40,7,10,17.9,35,46.6,60,75.4,340,145,70,85,40,0,'t02','array('id'=&gt;'t02','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Spearman','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'40','speed'=&gt;'7','offense'=&gt;'10','offense_max'=&gt;'17.9','defense_inf'=&gt;'35','defense_inf_max'=&gt;'46.6','defense_cav'=&gt;'60','defense_cav_max'=&gt;'75.4','cost'=&gt;'340','cost_wood'=&gt;'145','cost_clay'=&gt;'70','cost_iron'=&gt;'85','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'t02'),');</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -2136,12 +2026,17 @@
       <c r="T14" s="3">
         <v>0</v>
       </c>
-      <c r="U14" t="s">
-        <v>173</v>
+      <c r="U14" t="str">
+        <f t="shared" si="0"/>
+        <v>t03</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t03','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Axeman','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'6','offense'=&gt;'60','offense_max'=&gt;'75.4','defense_inf'=&gt;'30','defense_inf_max'=&gt;'40.9','defense_cav'=&gt;'30','defense_cav_max'=&gt;'40.9','cost'=&gt;'490','cost_wood'=&gt;'130','cost_clay'=&gt;'120','cost_iron'=&gt;'170','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'t03'),</v>
       </c>
       <c r="W14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t03','Teuton',2,'Axeman',1,1,50,6,60,75.4,30,40.9,30,40.9,490,130,120,170,70,0,'t03.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t03','Teuton',2,'Axeman',1,1,50,6,60,75.4,30,40.9,30,40.9,490,130,120,170,70,0,'t03','array('id'=&gt;'t03','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Axeman','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'6','offense'=&gt;'60','offense_max'=&gt;'75.4','defense_inf'=&gt;'30','defense_inf_max'=&gt;'40.9','defense_cav'=&gt;'30','defense_cav_max'=&gt;'40.9','cost'=&gt;'490','cost_wood'=&gt;'130','cost_clay'=&gt;'120','cost_iron'=&gt;'170','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'t03'),');</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -2205,12 +2100,17 @@
       <c r="T15" s="3">
         <v>0</v>
       </c>
-      <c r="U15" t="s">
-        <v>174</v>
+      <c r="U15" t="str">
+        <f t="shared" si="0"/>
+        <v>t04</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t04','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Scout','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'9','offense'=&gt;'0','offense_max'=&gt;'6.4','defense_inf'=&gt;'10','defense_inf_max'=&gt;'17.9','defense_cav'=&gt;'5','defense_cav_max'=&gt;'12.1','cost'=&gt;'360','cost_wood'=&gt;'160','cost_clay'=&gt;'100','cost_iron'=&gt;'50','cost_crop'=&gt;'50','time'=&gt;'0','image'=&gt;'t04'),</v>
       </c>
       <c r="W15" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t04','Teuton',2,'Scout',0,1,0,9,0,6.4,10,17.9,5,12.1,360,160,100,50,50,0,'t04.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t04','Teuton',2,'Scout',0,1,0,9,0,6.4,10,17.9,5,12.1,360,160,100,50,50,0,'t04','array('id'=&gt;'t04','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Scout','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'9','offense'=&gt;'0','offense_max'=&gt;'6.4','defense_inf'=&gt;'10','defense_inf_max'=&gt;'17.9','defense_cav'=&gt;'5','defense_cav_max'=&gt;'12.1','cost'=&gt;'360','cost_wood'=&gt;'160','cost_clay'=&gt;'100','cost_iron'=&gt;'50','cost_crop'=&gt;'50','time'=&gt;'0','image'=&gt;'t04'),');</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
@@ -2274,12 +2174,17 @@
       <c r="T16" s="3">
         <v>0</v>
       </c>
-      <c r="U16" t="s">
-        <v>175</v>
+      <c r="U16" t="str">
+        <f t="shared" si="0"/>
+        <v>t05</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t05','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Paladin','type'=&gt;'5','upkeep'=&gt;'2','carry'=&gt;'110','speed'=&gt;'10','offense'=&gt;'55','offense_max'=&gt;'76','defense_inf'=&gt;'100','defense_inf_max'=&gt;'127.7','defense_cav'=&gt;'40','defense_cav_max'=&gt;'58.7','cost'=&gt;'1005','cost_wood'=&gt;'370','cost_clay'=&gt;'270','cost_iron'=&gt;'290','cost_crop'=&gt;'75','time'=&gt;'0','image'=&gt;'t05'),</v>
       </c>
       <c r="W16" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t05','Teuton',2,'Paladin',5,2,110,10,55,76,100,127.7,40,58.7,1005,370,270,290,75,0,'t05.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t05','Teuton',2,'Paladin',5,2,110,10,55,76,100,127.7,40,58.7,1005,370,270,290,75,0,'t05','array('id'=&gt;'t05','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Paladin','type'=&gt;'5','upkeep'=&gt;'2','carry'=&gt;'110','speed'=&gt;'10','offense'=&gt;'55','offense_max'=&gt;'76','defense_inf'=&gt;'100','defense_inf_max'=&gt;'127.7','defense_cav'=&gt;'40','defense_cav_max'=&gt;'58.7','cost'=&gt;'1005','cost_wood'=&gt;'370','cost_clay'=&gt;'270','cost_iron'=&gt;'290','cost_crop'=&gt;'75','time'=&gt;'0','image'=&gt;'t05'),');</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
@@ -2343,12 +2248,17 @@
       <c r="T17" s="3">
         <v>0</v>
       </c>
-      <c r="U17" t="s">
-        <v>176</v>
+      <c r="U17" t="str">
+        <f t="shared" si="0"/>
+        <v>t06</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t06','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Teutonic Knight','type'=&gt;'7','upkeep'=&gt;'3','carry'=&gt;'80','speed'=&gt;'9','offense'=&gt;'150','offense_max'=&gt;'191.6','defense_inf'=&gt;'50','defense_inf_max'=&gt;'76.6','defense_cav'=&gt;'75','defense_cav_max'=&gt;'105.3','cost'=&gt;'1525','cost_wood'=&gt;'450','cost_clay'=&gt;'515','cost_iron'=&gt;'480','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'t06'),</v>
       </c>
       <c r="W17" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t06','Teuton',2,'Teutonic Knight',7,3,80,9,150,191.6,50,76.6,75,105.3,1525,450,515,480,80,0,'t06.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t06','Teuton',2,'Teutonic Knight',7,3,80,9,150,191.6,50,76.6,75,105.3,1525,450,515,480,80,0,'t06','array('id'=&gt;'t06','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Teutonic Knight','type'=&gt;'7','upkeep'=&gt;'3','carry'=&gt;'80','speed'=&gt;'9','offense'=&gt;'150','offense_max'=&gt;'191.6','defense_inf'=&gt;'50','defense_inf_max'=&gt;'76.6','defense_cav'=&gt;'75','defense_cav_max'=&gt;'105.3','cost'=&gt;'1525','cost_wood'=&gt;'450','cost_clay'=&gt;'515','cost_iron'=&gt;'480','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'t06'),');</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
@@ -2412,12 +2322,17 @@
       <c r="T18" s="3">
         <v>0</v>
       </c>
-      <c r="U18" t="s">
-        <v>177</v>
+      <c r="U18" t="str">
+        <f t="shared" si="0"/>
+        <v>t07</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t07','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'65','offense_max'=&gt;'93.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'80','defense_cav_max'=&gt;'111.1','cost'=&gt;'1720','cost_wood'=&gt;'1000','cost_clay'=&gt;'300','cost_iron'=&gt;'350','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'t07'),</v>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t07','Teuton',2,'Ram',6,3,0,4,65,93.9,30,53.6,80,111.1,1720,1000,300,350,70,0,'t07.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t07','Teuton',2,'Ram',6,3,0,4,65,93.9,30,53.6,80,111.1,1720,1000,300,350,70,0,'t07','array('id'=&gt;'t07','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'65','offense_max'=&gt;'93.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'80','defense_cav_max'=&gt;'111.1','cost'=&gt;'1720','cost_wood'=&gt;'1000','cost_clay'=&gt;'300','cost_iron'=&gt;'350','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'t07'),');</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
@@ -2481,12 +2396,17 @@
       <c r="T19" s="3">
         <v>0</v>
       </c>
-      <c r="U19" t="s">
-        <v>178</v>
+      <c r="U19" t="str">
+        <f t="shared" si="0"/>
+        <v>t08</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t08','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'50','offense_max'=&gt;'95.7','defense_inf'=&gt;'60','defense_inf_max'=&gt;'107.2','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'2760','cost_wood'=&gt;'900','cost_clay'=&gt;'1200','cost_iron'=&gt;'600','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'t08'),</v>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t08','Teuton',2,'Catapult',6,6,0,3,50,95.7,60,107.2,10,49.7,2760,900,1200,600,60,0,'t08.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t08','Teuton',2,'Catapult',6,6,0,3,50,95.7,60,107.2,10,49.7,2760,900,1200,600,60,0,'t08','array('id'=&gt;'t08','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'50','offense_max'=&gt;'95.7','defense_inf'=&gt;'60','defense_inf_max'=&gt;'107.2','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'2760','cost_wood'=&gt;'900','cost_clay'=&gt;'1200','cost_iron'=&gt;'600','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'t08'),');</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
@@ -2550,12 +2470,17 @@
       <c r="T20" s="3">
         <v>0</v>
       </c>
-      <c r="U20" t="s">
-        <v>179</v>
+      <c r="U20" t="str">
+        <f t="shared" si="0"/>
+        <v>t09</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t09','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Chief','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'60','defense_inf_max'=&gt;'60','defense_cav'=&gt;'40','defense_cav_max'=&gt;'40','cost'=&gt;'114300','cost_wood'=&gt;'35500','cost_clay'=&gt;'26600','cost_iron'=&gt;'25000','cost_crop'=&gt;'27200','time'=&gt;'0','image'=&gt;'t09'),</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t09','Teuton',2,'Chief',8,4,0,4,40,40,60,60,40,40,114300,35500,26600,25000,27200,0,'t09.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t09','Teuton',2,'Chief',8,4,0,4,40,40,60,60,40,40,114300,35500,26600,25000,27200,0,'t09','array('id'=&gt;'t09','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Chief','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'60','defense_inf_max'=&gt;'60','defense_cav'=&gt;'40','defense_cav_max'=&gt;'40','cost'=&gt;'114300','cost_wood'=&gt;'35500','cost_clay'=&gt;'26600','cost_iron'=&gt;'25000','cost_crop'=&gt;'27200','time'=&gt;'0','image'=&gt;'t09'),');</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
@@ -2619,12 +2544,17 @@
       <c r="T21" s="3">
         <v>0</v>
       </c>
-      <c r="U21" t="s">
-        <v>180</v>
+      <c r="U21" t="str">
+        <f t="shared" si="0"/>
+        <v>t10</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'t10','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'10','offense_max'=&gt;'10','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'20000','cost_wood'=&gt;'5800','cost_clay'=&gt;'4400','cost_iron'=&gt;'4600','cost_crop'=&gt;'5200','time'=&gt;'0','image'=&gt;'t10'),</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('t10','Teuton',2,'Settler',8,1,3000,5,10,10,80,80,80,80,20000,5800,4400,4600,5200,0,'t10.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('t10','Teuton',2,'Settler',8,1,3000,5,10,10,80,80,80,80,20000,5800,4400,4600,5200,0,'t10','array('id'=&gt;'t10','tribe'=&gt;'Teuton','tribe_id'=&gt;'2','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'10','offense_max'=&gt;'10','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'20000','cost_wood'=&gt;'5800','cost_clay'=&gt;'4400','cost_iron'=&gt;'4600','cost_crop'=&gt;'5200','time'=&gt;'0','image'=&gt;'t10'),');</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
@@ -2688,12 +2618,17 @@
       <c r="T22" s="3">
         <v>0</v>
       </c>
-      <c r="U22" t="s">
-        <v>181</v>
+      <c r="U22" t="str">
+        <f t="shared" si="0"/>
+        <v>g01</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g01','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Phalanx','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'35','speed'=&gt;'7','offense'=&gt;'15','offense_max'=&gt;'23.6','defense_inf'=&gt;'40','defense_inf_max'=&gt;'52.4','defense_cav'=&gt;'50','defense_cav_max'=&gt;'63.9','cost'=&gt;'315','cost_wood'=&gt;'100','cost_clay'=&gt;'130','cost_iron'=&gt;'55','cost_crop'=&gt;'30','time'=&gt;'0','image'=&gt;'g01'),</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g01','Gaul',3,'Phalanx',1,1,35,7,15,23.6,40,52.4,50,63.9,315,100,130,55,30,0,'g01.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g01','Gaul',3,'Phalanx',1,1,35,7,15,23.6,40,52.4,50,63.9,315,100,130,55,30,0,'g01','array('id'=&gt;'g01','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Phalanx','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'35','speed'=&gt;'7','offense'=&gt;'15','offense_max'=&gt;'23.6','defense_inf'=&gt;'40','defense_inf_max'=&gt;'52.4','defense_cav'=&gt;'50','defense_cav_max'=&gt;'63.9','cost'=&gt;'315','cost_wood'=&gt;'100','cost_clay'=&gt;'130','cost_iron'=&gt;'55','cost_crop'=&gt;'30','time'=&gt;'0','image'=&gt;'g01'),');</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
@@ -2757,12 +2692,17 @@
       <c r="T23" s="3">
         <v>0</v>
       </c>
-      <c r="U23" t="s">
-        <v>182</v>
+      <c r="U23" t="str">
+        <f t="shared" si="0"/>
+        <v>g02</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g02','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Swordsman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'45','speed'=&gt;'6','offense'=&gt;'65','offense_max'=&gt;'81.1','defense_inf'=&gt;'35','defense_inf_max'=&gt;'46.6','defense_cav'=&gt;'20','defense_cav_max'=&gt;'29.4','cost'=&gt;'535','cost_wood'=&gt;'140','cost_clay'=&gt;'150','cost_iron'=&gt;'185','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'g02'),</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g02','Gaul',3,'Swordsman',2,1,45,6,65,81.1,35,46.6,20,29.4,535,140,150,185,60,0,'g02.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g02','Gaul',3,'Swordsman',2,1,45,6,65,81.1,35,46.6,20,29.4,535,140,150,185,60,0,'g02','array('id'=&gt;'g02','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Swordsman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'45','speed'=&gt;'6','offense'=&gt;'65','offense_max'=&gt;'81.1','defense_inf'=&gt;'35','defense_inf_max'=&gt;'46.6','defense_cav'=&gt;'20','defense_cav_max'=&gt;'29.4','cost'=&gt;'535','cost_wood'=&gt;'140','cost_clay'=&gt;'150','cost_iron'=&gt;'185','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'g02'),');</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
@@ -2826,12 +2766,17 @@
       <c r="T24" s="3">
         <v>0</v>
       </c>
-      <c r="U24" t="s">
-        <v>183</v>
+      <c r="U24" t="str">
+        <f t="shared" si="0"/>
+        <v>g03</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g03','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Pathfinder','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'17','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'380','cost_wood'=&gt;'170','cost_clay'=&gt;'150','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'g03'),</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g03','Gaul',3,'Pathfinder',0,2,0,17,0,12.7,20,35.7,10,24.2,380,170,150,20,40,0,'g03.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g03','Gaul',3,'Pathfinder',0,2,0,17,0,12.7,20,35.7,10,24.2,380,170,150,20,40,0,'g03','array('id'=&gt;'g03','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Pathfinder','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'17','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'380','cost_wood'=&gt;'170','cost_clay'=&gt;'150','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'g03'),');</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
@@ -2895,12 +2840,17 @@
       <c r="T25" s="3">
         <v>0</v>
       </c>
-      <c r="U25" t="s">
-        <v>184</v>
+      <c r="U25" t="str">
+        <f t="shared" si="0"/>
+        <v>g04</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g04','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Theutates Thunder','type'=&gt;'4','upkeep'=&gt;'2','carry'=&gt;'75','speed'=&gt;'19','offense'=&gt;'90','offense_max'=&gt;'116.2','defense_inf'=&gt;'25','defense_inf_max'=&gt;'41.5','defense_cav'=&gt;'40','defense_cav_max'=&gt;'58.7','cost'=&gt;'1090','cost_wood'=&gt;'350','cost_clay'=&gt;'450','cost_iron'=&gt;'230','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'g04'),</v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g04','Gaul',3,'Theutates Thunder',4,2,75,19,90,116.2,25,41.5,40,58.7,1090,350,450,230,60,0,'g04.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g04','Gaul',3,'Theutates Thunder',4,2,75,19,90,116.2,25,41.5,40,58.7,1090,350,450,230,60,0,'g04','array('id'=&gt;'g04','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Theutates Thunder','type'=&gt;'4','upkeep'=&gt;'2','carry'=&gt;'75','speed'=&gt;'19','offense'=&gt;'90','offense_max'=&gt;'116.2','defense_inf'=&gt;'25','defense_inf_max'=&gt;'41.5','defense_cav'=&gt;'40','defense_cav_max'=&gt;'58.7','cost'=&gt;'1090','cost_wood'=&gt;'350','cost_clay'=&gt;'450','cost_iron'=&gt;'230','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'g04'),');</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
@@ -2964,12 +2914,17 @@
       <c r="T26" s="3">
         <v>0</v>
       </c>
-      <c r="U26" t="s">
-        <v>185</v>
+      <c r="U26" t="str">
+        <f t="shared" si="0"/>
+        <v>g05</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g05','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Druidrider','type'=&gt;'5','upkeep'=&gt;'2','carry'=&gt;'35','speed'=&gt;'16','offense'=&gt;'45','offense_max'=&gt;'64.5','defense_inf'=&gt;'115','defense_inf_max'=&gt;'145','defense_cav'=&gt;'55','defense_cav_max'=&gt;'76','cost'=&gt;'1090','cost_wood'=&gt;'360','cost_clay'=&gt;'330','cost_iron'=&gt;'280','cost_crop'=&gt;'120','time'=&gt;'0','image'=&gt;'g05'),</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g05','Gaul',3,'Druidrider',5,2,35,16,45,64.5,115,145,55,76,1090,360,330,280,120,0,'g05.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g05','Gaul',3,'Druidrider',5,2,35,16,45,64.5,115,145,55,76,1090,360,330,280,120,0,'g05','array('id'=&gt;'g05','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Druidrider','type'=&gt;'5','upkeep'=&gt;'2','carry'=&gt;'35','speed'=&gt;'16','offense'=&gt;'45','offense_max'=&gt;'64.5','defense_inf'=&gt;'115','defense_inf_max'=&gt;'145','defense_cav'=&gt;'55','defense_cav_max'=&gt;'76','cost'=&gt;'1090','cost_wood'=&gt;'360','cost_clay'=&gt;'330','cost_iron'=&gt;'280','cost_crop'=&gt;'120','time'=&gt;'0','image'=&gt;'g05'),');</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
@@ -3033,12 +2988,17 @@
       <c r="T27" s="3">
         <v>0</v>
       </c>
-      <c r="U27" t="s">
-        <v>186</v>
+      <c r="U27" t="str">
+        <f t="shared" si="0"/>
+        <v>g06</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g06','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Haeduan','type'=&gt;'7','upkeep'=&gt;'3','carry'=&gt;'65','speed'=&gt;'13','offense'=&gt;'140','offense_max'=&gt;'180.1','defense_inf'=&gt;'60','defense_inf_max'=&gt;'88.1','defense_cav'=&gt;'165','defense_cav_max'=&gt;'208.8','cost'=&gt;'1965','cost_wood'=&gt;'500','cost_clay'=&gt;'620','cost_iron'=&gt;'675','cost_crop'=&gt;'170','time'=&gt;'0','image'=&gt;'g06'),</v>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g06','Gaul',3,'Haeduan',7,3,65,13,140,180.1,60,88.1,165,208.8,1965,500,620,675,170,0,'g06.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g06','Gaul',3,'Haeduan',7,3,65,13,140,180.1,60,88.1,165,208.8,1965,500,620,675,170,0,'g06','array('id'=&gt;'g06','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Haeduan','type'=&gt;'7','upkeep'=&gt;'3','carry'=&gt;'65','speed'=&gt;'13','offense'=&gt;'140','offense_max'=&gt;'180.1','defense_inf'=&gt;'60','defense_inf_max'=&gt;'88.1','defense_cav'=&gt;'165','defense_cav_max'=&gt;'208.8','cost'=&gt;'1965','cost_wood'=&gt;'500','cost_clay'=&gt;'620','cost_iron'=&gt;'675','cost_crop'=&gt;'170','time'=&gt;'0','image'=&gt;'g06'),');</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
@@ -3102,12 +3062,17 @@
       <c r="T28" s="3">
         <v>0</v>
       </c>
-      <c r="U28" t="s">
-        <v>187</v>
+      <c r="U28" t="str">
+        <f t="shared" si="0"/>
+        <v>g07</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g07','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'50','offense_max'=&gt;'76.6','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'105','defense_cav_max'=&gt;'139.8','cost'=&gt;'1910','cost_wood'=&gt;'950','cost_clay'=&gt;'555','cost_iron'=&gt;'330','cost_crop'=&gt;'75','time'=&gt;'0','image'=&gt;'g07'),</v>
       </c>
       <c r="W28" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g07','Gaul',3,'Ram',6,3,0,4,50,76.6,30,53.6,105,139.8,1910,950,555,330,75,0,'g07.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g07','Gaul',3,'Ram',6,3,0,4,50,76.6,30,53.6,105,139.8,1910,950,555,330,75,0,'g07','array('id'=&gt;'g07','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'50','offense_max'=&gt;'76.6','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'105','defense_cav_max'=&gt;'139.8','cost'=&gt;'1910','cost_wood'=&gt;'950','cost_clay'=&gt;'555','cost_iron'=&gt;'330','cost_crop'=&gt;'75','time'=&gt;'0','image'=&gt;'g07'),');</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
@@ -3171,12 +3136,17 @@
       <c r="T29" s="3">
         <v>0</v>
       </c>
-      <c r="U29" t="s">
-        <v>188</v>
+      <c r="U29" t="str">
+        <f t="shared" si="0"/>
+        <v>g08</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g08','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Trebuchet','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'70','offense_max'=&gt;'118.7','defense_inf'=&gt;'45','defense_inf_max'=&gt;'90','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'3130','cost_wood'=&gt;'960','cost_clay'=&gt;'1450','cost_iron'=&gt;'630','cost_crop'=&gt;'90','time'=&gt;'0','image'=&gt;'g08'),</v>
       </c>
       <c r="W29" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g08','Gaul',3,'Trebuchet',6,6,0,3,70,118.7,45,90,10,49.7,3130,960,1450,630,90,0,'g08.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g08','Gaul',3,'Trebuchet',6,6,0,3,70,118.7,45,90,10,49.7,3130,960,1450,630,90,0,'g08','array('id'=&gt;'g08','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Trebuchet','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'70','offense_max'=&gt;'118.7','defense_inf'=&gt;'45','defense_inf_max'=&gt;'90','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'3130','cost_wood'=&gt;'960','cost_clay'=&gt;'1450','cost_iron'=&gt;'630','cost_crop'=&gt;'90','time'=&gt;'0','image'=&gt;'g08'),');</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
@@ -3240,12 +3210,17 @@
       <c r="T30" s="3">
         <v>0</v>
       </c>
-      <c r="U30" t="s">
-        <v>189</v>
+      <c r="U30" t="str">
+        <f t="shared" si="0"/>
+        <v>g09</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g09','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Chieftain','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'144650','cost_wood'=&gt;'30750','cost_clay'=&gt;'45400','cost_iron'=&gt;'31000','cost_crop'=&gt;'37500','time'=&gt;'0','image'=&gt;'g09'),</v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g09','Gaul',3,'Chieftain',8,4,0,5,40,40,50,50,50,50,144650,30750,45400,31000,37500,0,'g09.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g09','Gaul',3,'Chieftain',8,4,0,5,40,40,50,50,50,50,144650,30750,45400,31000,37500,0,'g09','array('id'=&gt;'g09','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Chieftain','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'144650','cost_wood'=&gt;'30750','cost_clay'=&gt;'45400','cost_iron'=&gt;'31000','cost_crop'=&gt;'37500','time'=&gt;'0','image'=&gt;'g09'),');</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -3309,12 +3284,17 @@
       <c r="T31" s="3">
         <v>0</v>
       </c>
-      <c r="U31" t="s">
-        <v>190</v>
+      <c r="U31" t="str">
+        <f t="shared" si="0"/>
+        <v>g10</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'g10','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'18100','cost_wood'=&gt;'4400','cost_clay'=&gt;'5600','cost_iron'=&gt;'4200','cost_crop'=&gt;'3900','time'=&gt;'0','image'=&gt;'g10'),</v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('g10','Gaul',3,'Settler',8,1,3000,5,0,0,80,80,80,80,18100,4400,5600,4200,3900,0,'g10.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('g10','Gaul',3,'Settler',8,1,3000,5,0,0,80,80,80,80,18100,4400,5600,4200,3900,0,'g10','array('id'=&gt;'g10','tribe'=&gt;'Gaul','tribe_id'=&gt;'3','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'18100','cost_wood'=&gt;'4400','cost_clay'=&gt;'5600','cost_iron'=&gt;'4200','cost_crop'=&gt;'3900','time'=&gt;'0','image'=&gt;'g10'),');</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
@@ -3378,12 +3358,17 @@
       <c r="T32" s="3">
         <v>0</v>
       </c>
-      <c r="U32" t="s">
-        <v>191</v>
+      <c r="U32" t="str">
+        <f t="shared" si="0"/>
+        <v>a01</v>
+      </c>
+      <c r="V32" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a01','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Rat','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'10','offense_max'=&gt;'10','defense_inf'=&gt;'25','defense_inf_max'=&gt;'25','defense_cav'=&gt;'20','defense_cav_max'=&gt;'20','cost'=&gt;'100','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'100','time'=&gt;'0','image'=&gt;'a01'),</v>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a01','Nature',4,'Rat',0,1,0,20,10,10,25,25,20,20,100,0,0,0,100,0,'a01.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a01','Nature',4,'Rat',0,1,0,20,10,10,25,25,20,20,100,0,0,0,100,0,'a01','array('id'=&gt;'a01','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Rat','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'10','offense_max'=&gt;'10','defense_inf'=&gt;'25','defense_inf_max'=&gt;'25','defense_cav'=&gt;'20','defense_cav_max'=&gt;'20','cost'=&gt;'100','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'100','time'=&gt;'0','image'=&gt;'a01'),');</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
@@ -3447,12 +3432,17 @@
       <c r="T33" s="3">
         <v>0</v>
       </c>
-      <c r="U33" t="s">
-        <v>192</v>
+      <c r="U33" t="str">
+        <f t="shared" si="0"/>
+        <v>a02</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a02','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Spider','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'20','offense_max'=&gt;'20','defense_inf'=&gt;'35','defense_inf_max'=&gt;'35','defense_cav'=&gt;'40','defense_cav_max'=&gt;'40','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a02'),</v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a02','Nature',4,'Spider',0,1,0,20,20,20,35,35,40,40,0,0,0,0,0,0,'a02.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a02','Nature',4,'Spider',0,1,0,20,20,20,35,35,40,40,0,0,0,0,0,0,'a02','array('id'=&gt;'a02','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Spider','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'20','offense_max'=&gt;'20','defense_inf'=&gt;'35','defense_inf_max'=&gt;'35','defense_cav'=&gt;'40','defense_cav_max'=&gt;'40','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a02'),');</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
@@ -3516,12 +3506,17 @@
       <c r="T34" s="3">
         <v>0</v>
       </c>
-      <c r="U34" t="s">
-        <v>193</v>
+      <c r="U34" t="str">
+        <f t="shared" si="0"/>
+        <v>a03</v>
+      </c>
+      <c r="V34" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a03','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Serpent','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'60','offense_max'=&gt;'60','defense_inf'=&gt;'40','defense_inf_max'=&gt;'40','defense_cav'=&gt;'60','defense_cav_max'=&gt;'60','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a03'),</v>
       </c>
       <c r="W34" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a03','Nature',4,'Serpent',0,1,0,20,60,60,40,40,60,60,0,0,0,0,0,0,'a03.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a03','Nature',4,'Serpent',0,1,0,20,60,60,40,40,60,60,0,0,0,0,0,0,'a03','array('id'=&gt;'a03','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Serpent','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'60','offense_max'=&gt;'60','defense_inf'=&gt;'40','defense_inf_max'=&gt;'40','defense_cav'=&gt;'60','defense_cav_max'=&gt;'60','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a03'),');</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
@@ -3585,12 +3580,17 @@
       <c r="T35" s="3">
         <v>0</v>
       </c>
-      <c r="U35" t="s">
-        <v>194</v>
+      <c r="U35" t="str">
+        <f t="shared" si="0"/>
+        <v>a04</v>
+      </c>
+      <c r="V35" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a04','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Bat','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'80','offense_max'=&gt;'80','defense_inf'=&gt;'66','defense_inf_max'=&gt;'66','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a04'),</v>
       </c>
       <c r="W35" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a04','Nature',4,'Bat',0,1,0,20,80,80,66,66,50,50,0,0,0,0,0,0,'a04.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a04','Nature',4,'Bat',0,1,0,20,80,80,66,66,50,50,0,0,0,0,0,0,'a04','array('id'=&gt;'a04','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Bat','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'80','offense_max'=&gt;'80','defense_inf'=&gt;'66','defense_inf_max'=&gt;'66','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a04'),');</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
@@ -3654,12 +3654,17 @@
       <c r="T36" s="3">
         <v>0</v>
       </c>
-      <c r="U36" t="s">
-        <v>195</v>
+      <c r="U36" t="str">
+        <f t="shared" si="0"/>
+        <v>a05</v>
+      </c>
+      <c r="V36" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a05','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Wild boar','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'50','offense_max'=&gt;'50','defense_inf'=&gt;'70','defense_inf_max'=&gt;'70','defense_cav'=&gt;'33','defense_cav_max'=&gt;'33','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a05'),</v>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a05','Nature',4,'Wild boar',0,2,0,20,50,50,70,70,33,33,0,0,0,0,0,0,'a05.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a05','Nature',4,'Wild boar',0,2,0,20,50,50,70,70,33,33,0,0,0,0,0,0,'a05','array('id'=&gt;'a05','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Wild boar','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'50','offense_max'=&gt;'50','defense_inf'=&gt;'70','defense_inf_max'=&gt;'70','defense_cav'=&gt;'33','defense_cav_max'=&gt;'33','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a05'),');</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
@@ -3723,12 +3728,17 @@
       <c r="T37" s="3">
         <v>0</v>
       </c>
-      <c r="U37" t="s">
-        <v>196</v>
+      <c r="U37" t="str">
+        <f t="shared" si="0"/>
+        <v>a06</v>
+      </c>
+      <c r="V37" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a06','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Wolf','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'100','offense_max'=&gt;'100','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'70','defense_cav_max'=&gt;'70','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a06'),</v>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a06','Nature',4,'Wolf',0,2,0,20,100,100,80,80,70,70,0,0,0,0,0,0,'a06.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a06','Nature',4,'Wolf',0,2,0,20,100,100,80,80,70,70,0,0,0,0,0,0,'a06','array('id'=&gt;'a06','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Wolf','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'100','offense_max'=&gt;'100','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'70','defense_cav_max'=&gt;'70','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a06'),');</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.3">
@@ -3792,12 +3802,17 @@
       <c r="T38" s="3">
         <v>0</v>
       </c>
-      <c r="U38" t="s">
-        <v>197</v>
+      <c r="U38" t="str">
+        <f t="shared" si="0"/>
+        <v>a07</v>
+      </c>
+      <c r="V38" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a07','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Bear','type'=&gt;'0','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'250','offense_max'=&gt;'250','defense_inf'=&gt;'140','defense_inf_max'=&gt;'140','defense_cav'=&gt;'200','defense_cav_max'=&gt;'200','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a07'),</v>
       </c>
       <c r="W38" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a07','Nature',4,'Bear',0,3,0,20,250,250,140,140,200,200,0,0,0,0,0,0,'a07.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a07','Nature',4,'Bear',0,3,0,20,250,250,140,140,200,200,0,0,0,0,0,0,'a07','array('id'=&gt;'a07','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Bear','type'=&gt;'0','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'250','offense_max'=&gt;'250','defense_inf'=&gt;'140','defense_inf_max'=&gt;'140','defense_cav'=&gt;'200','defense_cav_max'=&gt;'200','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a07'),');</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
@@ -3861,12 +3876,17 @@
       <c r="T39" s="3">
         <v>0</v>
       </c>
-      <c r="U39" t="s">
-        <v>198</v>
+      <c r="U39" t="str">
+        <f t="shared" si="0"/>
+        <v>a08</v>
+      </c>
+      <c r="V39" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a08','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Crocodile','type'=&gt;'0','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'450','offense_max'=&gt;'450','defense_inf'=&gt;'380','defense_inf_max'=&gt;'380','defense_cav'=&gt;'240','defense_cav_max'=&gt;'240','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a08'),</v>
       </c>
       <c r="W39" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a08','Nature',4,'Crocodile',0,3,0,20,450,450,380,380,240,240,0,0,0,0,0,0,'a08.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a08','Nature',4,'Crocodile',0,3,0,20,450,450,380,380,240,240,0,0,0,0,0,0,'a08','array('id'=&gt;'a08','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Crocodile','type'=&gt;'0','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'450','offense_max'=&gt;'450','defense_inf'=&gt;'380','defense_inf_max'=&gt;'380','defense_cav'=&gt;'240','defense_cav_max'=&gt;'240','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a08'),');</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
@@ -3930,12 +3950,17 @@
       <c r="T40" s="3">
         <v>0</v>
       </c>
-      <c r="U40" t="s">
-        <v>199</v>
+      <c r="U40" t="str">
+        <f t="shared" si="0"/>
+        <v>a09</v>
+      </c>
+      <c r="V40" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a09','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Tiger','type'=&gt;'0','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'200','offense_max'=&gt;'200','defense_inf'=&gt;'170','defense_inf_max'=&gt;'170','defense_cav'=&gt;'250','defense_cav_max'=&gt;'250','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a09'),</v>
       </c>
       <c r="W40" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a09','Nature',4,'Tiger',0,3,0,20,200,200,170,170,250,250,0,0,0,0,0,0,'a09.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a09','Nature',4,'Tiger',0,3,0,20,200,200,170,170,250,250,0,0,0,0,0,0,'a09','array('id'=&gt;'a09','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Tiger','type'=&gt;'0','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'200','offense_max'=&gt;'200','defense_inf'=&gt;'170','defense_inf_max'=&gt;'170','defense_cav'=&gt;'250','defense_cav_max'=&gt;'250','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a09'),');</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
@@ -3999,12 +4024,17 @@
       <c r="T41" s="3">
         <v>0</v>
       </c>
-      <c r="U41" t="s">
-        <v>200</v>
+      <c r="U41" t="str">
+        <f t="shared" si="0"/>
+        <v>a10</v>
+      </c>
+      <c r="V41" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'a10','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Elephant','type'=&gt;'0','upkeep'=&gt;'5','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'600','offense_max'=&gt;'600','defense_inf'=&gt;'440','defense_inf_max'=&gt;'440','defense_cav'=&gt;'520','defense_cav_max'=&gt;'520','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a10'),</v>
       </c>
       <c r="W41" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('a10','Nature',4,'Elephant',0,5,0,20,600,600,440,440,520,520,0,0,0,0,0,0,'a10.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('a10','Nature',4,'Elephant',0,5,0,20,600,600,440,440,520,520,0,0,0,0,0,0,'a10','array('id'=&gt;'a10','tribe'=&gt;'Nature','tribe_id'=&gt;'4','name'=&gt;'Elephant','type'=&gt;'0','upkeep'=&gt;'5','carry'=&gt;'0','speed'=&gt;'20','offense'=&gt;'600','offense_max'=&gt;'600','defense_inf'=&gt;'440','defense_inf_max'=&gt;'440','defense_cav'=&gt;'520','defense_cav_max'=&gt;'520','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'a10'),');</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
@@ -4068,12 +4098,17 @@
       <c r="T42" s="3">
         <v>0</v>
       </c>
-      <c r="U42" t="s">
-        <v>201</v>
+      <c r="U42" t="str">
+        <f t="shared" si="0"/>
+        <v>n01</v>
+      </c>
+      <c r="V42" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n01','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Pikeman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'6','offense'=&gt;'20','offense_max'=&gt;'20','defense_inf'=&gt;'35','defense_inf_max'=&gt;'35','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n01'),</v>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n01','Natar',5,'Pikeman',2,1,0,6,20,20,35,35,50,50,0,0,0,0,0,0,'n01.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n01','Natar',5,'Pikeman',2,1,0,6,20,20,35,35,50,50,0,0,0,0,0,0,'n01','array('id'=&gt;'n01','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Pikeman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'6','offense'=&gt;'20','offense_max'=&gt;'20','defense_inf'=&gt;'35','defense_inf_max'=&gt;'35','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n01'),');</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
@@ -4137,12 +4172,17 @@
       <c r="T43" s="3">
         <v>0</v>
       </c>
-      <c r="U43" t="s">
-        <v>202</v>
+      <c r="U43" t="str">
+        <f t="shared" si="0"/>
+        <v>n02</v>
+      </c>
+      <c r="V43" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n02','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Thorned Warrior','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'7','offense'=&gt;'65','offense_max'=&gt;'65','defense_inf'=&gt;'30','defense_inf_max'=&gt;'30','defense_cav'=&gt;'10','defense_cav_max'=&gt;'10','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n02'),</v>
       </c>
       <c r="W43" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n02','Natar',5,'Thorned Warrior',1,1,0,7,65,65,30,30,10,10,0,0,0,0,0,0,'n02.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n02','Natar',5,'Thorned Warrior',1,1,0,7,65,65,30,30,10,10,0,0,0,0,0,0,'n02','array('id'=&gt;'n02','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Thorned Warrior','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'7','offense'=&gt;'65','offense_max'=&gt;'65','defense_inf'=&gt;'30','defense_inf_max'=&gt;'30','defense_cav'=&gt;'10','defense_cav_max'=&gt;'10','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n02'),');</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
@@ -4206,12 +4246,17 @@
       <c r="T44" s="3">
         <v>0</v>
       </c>
-      <c r="U44" t="s">
-        <v>203</v>
+      <c r="U44" t="str">
+        <f t="shared" si="0"/>
+        <v>n03</v>
+      </c>
+      <c r="V44" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n03','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Guardsman','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'6','offense'=&gt;'100','offense_max'=&gt;'100','defense_inf'=&gt;'90','defense_inf_max'=&gt;'90','defense_cav'=&gt;'75','defense_cav_max'=&gt;'75','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n03'),</v>
       </c>
       <c r="W44" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n03','Natar',5,'Guardsman',3,1,0,6,100,100,90,90,75,75,0,0,0,0,0,0,'n03.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n03','Natar',5,'Guardsman',3,1,0,6,100,100,90,90,75,75,0,0,0,0,0,0,'n03','array('id'=&gt;'n03','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Guardsman','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'6','offense'=&gt;'100','offense_max'=&gt;'100','defense_inf'=&gt;'90','defense_inf_max'=&gt;'90','defense_cav'=&gt;'75','defense_cav_max'=&gt;'75','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n03'),');</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.3">
@@ -4275,12 +4320,17 @@
       <c r="T45" s="3">
         <v>0</v>
       </c>
-      <c r="U45" t="s">
-        <v>204</v>
+      <c r="U45" t="str">
+        <f t="shared" si="0"/>
+        <v>n04</v>
+      </c>
+      <c r="V45" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n04','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Birds Of Prey','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'25','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'10','defense_inf_max'=&gt;'10','defense_cav'=&gt;'0','defense_cav_max'=&gt;'0','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n04'),</v>
       </c>
       <c r="W45" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n04','Natar',5,'Birds Of Prey',3,1,0,25,0,0,10,10,0,0,0,0,0,0,0,0,'n04.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n04','Natar',5,'Birds Of Prey',3,1,0,25,0,0,10,10,0,0,0,0,0,0,0,0,'n04','array('id'=&gt;'n04','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Birds Of Prey','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'25','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'10','defense_inf_max'=&gt;'10','defense_cav'=&gt;'0','defense_cav_max'=&gt;'0','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n04'),');</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.3">
@@ -4344,12 +4394,17 @@
       <c r="T46" s="3">
         <v>0</v>
       </c>
-      <c r="U46" t="s">
-        <v>205</v>
+      <c r="U46" t="str">
+        <f t="shared" si="0"/>
+        <v>n05</v>
+      </c>
+      <c r="V46" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n05','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Axerider','type'=&gt;'1','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'14','offense'=&gt;'155','offense_max'=&gt;'155','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n05'),</v>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n05','Natar',5,'Axerider',1,2,0,14,155,155,80,80,50,50,0,0,0,0,0,0,'n05.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n05','Natar',5,'Axerider',1,2,0,14,155,155,80,80,50,50,0,0,0,0,0,0,'n05','array('id'=&gt;'n05','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Axerider','type'=&gt;'1','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'14','offense'=&gt;'155','offense_max'=&gt;'155','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n05'),');</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.3">
@@ -4413,12 +4468,17 @@
       <c r="T47" s="3">
         <v>0</v>
       </c>
-      <c r="U47" t="s">
-        <v>206</v>
+      <c r="U47" t="str">
+        <f t="shared" si="0"/>
+        <v>n06</v>
+      </c>
+      <c r="V47" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n06','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Natarian Knight','type'=&gt;'1','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'12','offense'=&gt;'170','offense_max'=&gt;'170','defense_inf'=&gt;'140','defense_inf_max'=&gt;'140','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n06'),</v>
       </c>
       <c r="W47" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n06','Natar',5,'Natarian Knight',1,3,0,12,170,170,140,140,80,80,0,0,0,0,0,0,'n06.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n06','Natar',5,'Natarian Knight',1,3,0,12,170,170,140,140,80,80,0,0,0,0,0,0,'n06','array('id'=&gt;'n06','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Natarian Knight','type'=&gt;'1','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'12','offense'=&gt;'170','offense_max'=&gt;'170','defense_inf'=&gt;'140','defense_inf_max'=&gt;'140','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n06'),');</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
@@ -4482,12 +4542,17 @@
       <c r="T48" s="3">
         <v>0</v>
       </c>
-      <c r="U48" t="s">
-        <v>207</v>
+      <c r="U48" t="str">
+        <f t="shared" si="0"/>
+        <v>n07</v>
+      </c>
+      <c r="V48" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n07','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Warelephant','type'=&gt;'1','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'250','offense_max'=&gt;'250','defense_inf'=&gt;'120','defense_inf_max'=&gt;'120','defense_cav'=&gt;'150','defense_cav_max'=&gt;'150','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n07'),</v>
       </c>
       <c r="W48" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n07','Natar',5,'Warelephant',1,4,0,5,250,250,120,120,150,150,0,0,0,0,0,0,'n07.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n07','Natar',5,'Warelephant',1,4,0,5,250,250,120,120,150,150,0,0,0,0,0,0,'n07','array('id'=&gt;'n07','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Warelephant','type'=&gt;'1','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'250','offense_max'=&gt;'250','defense_inf'=&gt;'120','defense_inf_max'=&gt;'120','defense_cav'=&gt;'150','defense_cav_max'=&gt;'150','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n07'),');</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.3">
@@ -4551,12 +4616,17 @@
       <c r="T49" s="3">
         <v>0</v>
       </c>
-      <c r="U49" t="s">
-        <v>208</v>
+      <c r="U49" t="str">
+        <f t="shared" si="0"/>
+        <v>n08</v>
+      </c>
+      <c r="V49" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n08','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Ballista','type'=&gt;'1','upkeep'=&gt;'5','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'60','offense_max'=&gt;'60','defense_inf'=&gt;'45','defense_inf_max'=&gt;'45','defense_cav'=&gt;'10','defense_cav_max'=&gt;'10','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n08'),</v>
       </c>
       <c r="W49" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n08','Natar',5,'Ballista',1,5,0,3,60,60,45,45,10,10,0,0,0,0,0,0,'n08.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n08','Natar',5,'Ballista',1,5,0,3,60,60,45,45,10,10,0,0,0,0,0,0,'n08','array('id'=&gt;'n08','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Ballista','type'=&gt;'1','upkeep'=&gt;'5','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'60','offense_max'=&gt;'60','defense_inf'=&gt;'45','defense_inf_max'=&gt;'45','defense_cav'=&gt;'10','defense_cav_max'=&gt;'10','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n08'),');</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.3">
@@ -4620,12 +4690,17 @@
       <c r="T50" s="3">
         <v>0</v>
       </c>
-      <c r="U50" t="s">
-        <v>209</v>
+      <c r="U50" t="str">
+        <f t="shared" si="0"/>
+        <v>n09</v>
+      </c>
+      <c r="V50" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n09','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Natarian Emperor','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'80','offense_max'=&gt;'80','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n09'),</v>
       </c>
       <c r="W50" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n09','Natar',5,'Natarian Emperor',1,1,0,5,80,80,50,50,50,50,0,0,0,0,0,0,'n09.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n09','Natar',5,'Natarian Emperor',1,1,0,5,80,80,50,50,50,50,0,0,0,0,0,0,'n09','array('id'=&gt;'n09','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Natarian Emperor','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'80','offense_max'=&gt;'80','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n09'),');</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.3">
@@ -4689,12 +4764,17 @@
       <c r="T51" s="3">
         <v>0</v>
       </c>
-      <c r="U51" t="s">
-        <v>210</v>
+      <c r="U51" t="str">
+        <f t="shared" si="0"/>
+        <v>n10</v>
+      </c>
+      <c r="V51" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'n10','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Settler','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'30','offense_max'=&gt;'30','defense_inf'=&gt;'40','defense_inf_max'=&gt;'40','defense_cav'=&gt;'40','defense_cav_max'=&gt;'40','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n10'),</v>
       </c>
       <c r="W51" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('n10','Natar',5,'Settler',0,1,0,5,30,30,40,40,40,40,0,0,0,0,0,0,'n10.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('n10','Natar',5,'Settler',0,1,0,5,30,30,40,40,40,40,0,0,0,0,0,0,'n10','array('id'=&gt;'n10','tribe'=&gt;'Natar','tribe_id'=&gt;'5','name'=&gt;'Settler','type'=&gt;'0','upkeep'=&gt;'1','carry'=&gt;'0','speed'=&gt;'5','offense'=&gt;'30','offense_max'=&gt;'30','defense_inf'=&gt;'40','defense_inf_max'=&gt;'40','defense_cav'=&gt;'40','defense_cav_max'=&gt;'40','cost'=&gt;'0','cost_wood'=&gt;'0','cost_clay'=&gt;'0','cost_iron'=&gt;'0','cost_crop'=&gt;'0','time'=&gt;'0','image'=&gt;'n10'),');</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.3">
@@ -4758,12 +4838,17 @@
       <c r="T52" s="3">
         <v>0</v>
       </c>
-      <c r="U52" t="s">
-        <v>211</v>
+      <c r="U52" t="str">
+        <f t="shared" si="0"/>
+        <v>e01</v>
+      </c>
+      <c r="V52" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e01','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Slave Militia','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'15','speed'=&gt;'7','offense'=&gt;'10','offense_max'=&gt;'17.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'40.9','defense_cav'=&gt;'20','defense_cav_max'=&gt;'29.4','cost'=&gt;'150','cost_wood'=&gt;'45','cost_clay'=&gt;'60','cost_iron'=&gt;'30','cost_crop'=&gt;'15','time'=&gt;'0','image'=&gt;'e01'),</v>
       </c>
       <c r="W52" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e01','Egyptian',6,'Slave Militia',3,1,15,7,10,17.9,30,40.9,20,29.4,150,45,60,30,15,0,'e01.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e01','Egyptian',6,'Slave Militia',3,1,15,7,10,17.9,30,40.9,20,29.4,150,45,60,30,15,0,'e01','array('id'=&gt;'e01','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Slave Militia','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'15','speed'=&gt;'7','offense'=&gt;'10','offense_max'=&gt;'17.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'40.9','defense_cav'=&gt;'20','defense_cav_max'=&gt;'29.4','cost'=&gt;'150','cost_wood'=&gt;'45','cost_clay'=&gt;'60','cost_iron'=&gt;'30','cost_crop'=&gt;'15','time'=&gt;'0','image'=&gt;'e01'),');</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.3">
@@ -4827,12 +4912,17 @@
       <c r="T53" s="3">
         <v>0</v>
       </c>
-      <c r="U53" t="s">
-        <v>212</v>
+      <c r="U53" t="str">
+        <f t="shared" si="0"/>
+        <v>e02</v>
+      </c>
+      <c r="V53" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e02','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Ash Warden','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'6','offense'=&gt;'30','offense_max'=&gt;'40.9','defense_inf'=&gt;'55','defense_inf_max'=&gt;'69.6','defense_cav'=&gt;'40','defense_cav_max'=&gt;'52.4','cost'=&gt;'420','cost_wood'=&gt;'115','cost_clay'=&gt;'100','cost_iron'=&gt;'145','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'e02'),</v>
       </c>
       <c r="W53" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e02','Egyptian',6,'Ash Warden',1,1,50,6,30,40.9,55,69.6,40,52.4,420,115,100,145,60,0,'e02.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e02','Egyptian',6,'Ash Warden',1,1,50,6,30,40.9,55,69.6,40,52.4,420,115,100,145,60,0,'e02','array('id'=&gt;'e02','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Ash Warden','type'=&gt;'1','upkeep'=&gt;'1','carry'=&gt;'50','speed'=&gt;'6','offense'=&gt;'30','offense_max'=&gt;'40.9','defense_inf'=&gt;'55','defense_inf_max'=&gt;'69.6','defense_cav'=&gt;'40','defense_cav_max'=&gt;'52.4','cost'=&gt;'420','cost_wood'=&gt;'115','cost_clay'=&gt;'100','cost_iron'=&gt;'145','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'e02'),');</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.3">
@@ -4896,12 +4986,17 @@
       <c r="T54" s="3">
         <v>0</v>
       </c>
-      <c r="U54" t="s">
-        <v>213</v>
+      <c r="U54" t="str">
+        <f t="shared" si="0"/>
+        <v>e03</v>
+      </c>
+      <c r="V54" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e03','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Khopesh Warrior','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'45','speed'=&gt;'7','offense'=&gt;'65','offense_max'=&gt;'81.1','defense_inf'=&gt;'50','defense_inf_max'=&gt;'63.9','defense_cav'=&gt;'20','defense_cav_max'=&gt;'29.4','cost'=&gt;'650','cost_wood'=&gt;'170','cost_clay'=&gt;'180','cost_iron'=&gt;'220','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'e03'),</v>
       </c>
       <c r="W54" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e03','Egyptian',6,'Khopesh Warrior',2,1,45,7,65,81.1,50,63.9,20,29.4,650,170,180,220,80,0,'e03.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e03','Egyptian',6,'Khopesh Warrior',2,1,45,7,65,81.1,50,63.9,20,29.4,650,170,180,220,80,0,'e03','array('id'=&gt;'e03','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Khopesh Warrior','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'45','speed'=&gt;'7','offense'=&gt;'65','offense_max'=&gt;'81.1','defense_inf'=&gt;'50','defense_inf_max'=&gt;'63.9','defense_cav'=&gt;'20','defense_cav_max'=&gt;'29.4','cost'=&gt;'650','cost_wood'=&gt;'170','cost_clay'=&gt;'180','cost_iron'=&gt;'220','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'e03'),');</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.3">
@@ -4965,12 +5060,17 @@
       <c r="T55" s="3">
         <v>0</v>
       </c>
-      <c r="U55" t="s">
-        <v>214</v>
+      <c r="U55" t="str">
+        <f t="shared" si="0"/>
+        <v>e04</v>
+      </c>
+      <c r="V55" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e04','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Sopdu Explorer','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'16','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'380','cost_wood'=&gt;'170','cost_clay'=&gt;'150','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'e04'),</v>
       </c>
       <c r="W55" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e04','Egyptian',6,'Sopdu Explorer',0,2,0,16,0,12.7,20,35.7,10,24.2,380,170,150,20,40,0,'e04.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e04','Egyptian',6,'Sopdu Explorer',0,2,0,16,0,12.7,20,35.7,10,24.2,380,170,150,20,40,0,'e04','array('id'=&gt;'e04','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Sopdu Explorer','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'0','speed'=&gt;'16','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'380','cost_wood'=&gt;'170','cost_clay'=&gt;'150','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'e04'),');</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.3">
@@ -5034,12 +5134,17 @@
       <c r="T56" s="3">
         <v>0</v>
       </c>
-      <c r="U56" t="s">
-        <v>215</v>
+      <c r="U56" t="str">
+        <f t="shared" si="0"/>
+        <v>e05</v>
+      </c>
+      <c r="V56" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e05','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Anhur Guard','type'=&gt;'5','upkeep'=&gt;'2','carry'=&gt;'50','speed'=&gt;'15','offense'=&gt;'50','offense_max'=&gt;'70.2','defense_inf'=&gt;'110','defense_inf_max'=&gt;'139.2','defense_cav'=&gt;'50','defense_cav_max'=&gt;'70.2','cost'=&gt;'1090','cost_wood'=&gt;'360','cost_clay'=&gt;'330','cost_iron'=&gt;'280','cost_crop'=&gt;'120','time'=&gt;'0','image'=&gt;'e05'),</v>
       </c>
       <c r="W56" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e05','Egyptian',6,'Anhur Guard',5,2,50,15,50,70.2,110,139.2,50,70.2,1090,360,330,280,120,0,'e05.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e05','Egyptian',6,'Anhur Guard',5,2,50,15,50,70.2,110,139.2,50,70.2,1090,360,330,280,120,0,'e05','array('id'=&gt;'e05','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Anhur Guard','type'=&gt;'5','upkeep'=&gt;'2','carry'=&gt;'50','speed'=&gt;'15','offense'=&gt;'50','offense_max'=&gt;'70.2','defense_inf'=&gt;'110','defense_inf_max'=&gt;'139.2','defense_cav'=&gt;'50','defense_cav_max'=&gt;'70.2','cost'=&gt;'1090','cost_wood'=&gt;'360','cost_clay'=&gt;'330','cost_iron'=&gt;'280','cost_crop'=&gt;'120','time'=&gt;'0','image'=&gt;'e05'),');</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.3">
@@ -5103,12 +5208,17 @@
       <c r="T57" s="3">
         <v>0</v>
       </c>
-      <c r="U57" t="s">
-        <v>216</v>
+      <c r="U57" t="str">
+        <f t="shared" si="0"/>
+        <v>e06</v>
+      </c>
+      <c r="V57" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e06','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Resheph Chariot','type'=&gt;'7','upkeep'=&gt;'3','carry'=&gt;'70','speed'=&gt;'10','offense'=&gt;'110','offense_max'=&gt;'145.6','defense_inf'=&gt;'120','defense_inf_max'=&gt;'157.1','defense_cav'=&gt;'150','defense_cav_max'=&gt;'191.6','cost'=&gt;'1800','cost_wood'=&gt;'450','cost_clay'=&gt;'560','cost_iron'=&gt;'610','cost_crop'=&gt;'180','time'=&gt;'0','image'=&gt;'e06'),</v>
       </c>
       <c r="W57" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e06','Egyptian',6,'Resheph Chariot',7,3,70,10,110,145.6,120,157.1,150,191.6,1800,450,560,610,180,0,'e06.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e06','Egyptian',6,'Resheph Chariot',7,3,70,10,110,145.6,120,157.1,150,191.6,1800,450,560,610,180,0,'e06','array('id'=&gt;'e06','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Resheph Chariot','type'=&gt;'7','upkeep'=&gt;'3','carry'=&gt;'70','speed'=&gt;'10','offense'=&gt;'110','offense_max'=&gt;'145.6','defense_inf'=&gt;'120','defense_inf_max'=&gt;'157.1','defense_cav'=&gt;'150','defense_cav_max'=&gt;'191.6','cost'=&gt;'1800','cost_wood'=&gt;'450','cost_clay'=&gt;'560','cost_iron'=&gt;'610','cost_crop'=&gt;'180','time'=&gt;'0','image'=&gt;'e06'),');</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.3">
@@ -5172,12 +5282,17 @@
       <c r="T58" s="3">
         <v>0</v>
       </c>
-      <c r="U58" t="s">
-        <v>217</v>
+      <c r="U58" t="str">
+        <f t="shared" si="0"/>
+        <v>e07</v>
+      </c>
+      <c r="V58" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e07','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'55','offense_max'=&gt;'82.4','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'95','defense_cav_max'=&gt;'128.3','cost'=&gt;'1990','cost_wood'=&gt;'995','cost_clay'=&gt;'575','cost_iron'=&gt;'340','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'e07'),</v>
       </c>
       <c r="W58" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e07','Egyptian',6,'Ram',6,3,0,4,55,82.4,30,53.6,95,128.3,1990,995,575,340,80,0,'e07.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e07','Egyptian',6,'Ram',6,3,0,4,55,82.4,30,53.6,95,128.3,1990,995,575,340,80,0,'e07','array('id'=&gt;'e07','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'55','offense_max'=&gt;'82.4','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'95','defense_cav_max'=&gt;'128.3','cost'=&gt;'1990','cost_wood'=&gt;'995','cost_clay'=&gt;'575','cost_iron'=&gt;'340','cost_crop'=&gt;'80','time'=&gt;'0','image'=&gt;'e07'),');</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.3">
@@ -5241,12 +5356,17 @@
       <c r="T59" s="3">
         <v>0</v>
       </c>
-      <c r="U59" t="s">
-        <v>218</v>
+      <c r="U59" t="str">
+        <f t="shared" si="0"/>
+        <v>e08</v>
+      </c>
+      <c r="V59" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e08','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Stone Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'65','offense_max'=&gt;'113','defense_inf'=&gt;'55','defense_inf_max'=&gt;'101.5','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'3250','cost_wood'=&gt;'980','cost_clay'=&gt;'1510','cost_iron'=&gt;'660','cost_crop'=&gt;'100','time'=&gt;'0','image'=&gt;'e08'),</v>
       </c>
       <c r="W59" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e08','Egyptian',6,'Stone Catapult',6,6,0,3,65,113,55,101.5,10,49.7,3250,980,1510,660,100,0,'e08.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e08','Egyptian',6,'Stone Catapult',6,6,0,3,65,113,55,101.5,10,49.7,3250,980,1510,660,100,0,'e08','array('id'=&gt;'e08','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Stone Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'0','speed'=&gt;'3','offense'=&gt;'65','offense_max'=&gt;'113','defense_inf'=&gt;'55','defense_inf_max'=&gt;'101.5','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'3250','cost_wood'=&gt;'980','cost_clay'=&gt;'1510','cost_iron'=&gt;'660','cost_crop'=&gt;'100','time'=&gt;'0','image'=&gt;'e08'),');</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.3">
@@ -5310,12 +5430,17 @@
       <c r="T60" s="3">
         <v>0</v>
       </c>
-      <c r="U60" t="s">
-        <v>219</v>
+      <c r="U60" t="str">
+        <f t="shared" si="0"/>
+        <v>e09</v>
+      </c>
+      <c r="V60" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e09','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Nomarch','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'160000','cost_wood'=&gt;'34000','cost_clay'=&gt;'50000','cost_iron'=&gt;'34000','cost_crop'=&gt;'42000','time'=&gt;'0','image'=&gt;'e09'),</v>
       </c>
       <c r="W60" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e09','Egyptian',6,'Nomarch',8,4,0,4,40,40,50,50,50,50,160000,34000,50000,34000,42000,0,'e09.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e09','Egyptian',6,'Nomarch',8,4,0,4,40,40,50,50,50,50,160000,34000,50000,34000,42000,0,'e09','array('id'=&gt;'e09','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Nomarch','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'0','speed'=&gt;'4','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'160000','cost_wood'=&gt;'34000','cost_clay'=&gt;'50000','cost_iron'=&gt;'34000','cost_crop'=&gt;'42000','time'=&gt;'0','image'=&gt;'e09'),');</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.3">
@@ -5379,12 +5504,17 @@
       <c r="T61" s="3">
         <v>0</v>
       </c>
-      <c r="U61" t="s">
-        <v>220</v>
+      <c r="U61" t="str">
+        <f t="shared" si="0"/>
+        <v>e10</v>
+      </c>
+      <c r="V61" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'e10','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'19000','cost_wood'=&gt;'4560','cost_clay'=&gt;'5890','cost_iron'=&gt;'4370','cost_crop'=&gt;'4180','time'=&gt;'0','image'=&gt;'e10'),</v>
       </c>
       <c r="W61" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('e10','Egyptian',6,'Settler',8,1,3000,5,0,0,80,80,80,80,19000,4560,5890,4370,4180,0,'e10.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('e10','Egyptian',6,'Settler',8,1,3000,5,0,0,80,80,80,80,19000,4560,5890,4370,4180,0,'e10','array('id'=&gt;'e10','tribe'=&gt;'Egyptian','tribe_id'=&gt;'6','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'3000','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'19000','cost_wood'=&gt;'4560','cost_clay'=&gt;'5890','cost_iron'=&gt;'4370','cost_crop'=&gt;'4180','time'=&gt;'0','image'=&gt;'e10'),');</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.3">
@@ -5448,12 +5578,17 @@
       <c r="T62" s="3">
         <v>0</v>
       </c>
-      <c r="U62" t="s">
-        <v>221</v>
+      <c r="U62" t="str">
+        <f t="shared" si="0"/>
+        <v>h01</v>
+      </c>
+      <c r="V62" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'h01','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Mercenary','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'30','speed'=&gt;'6','offense'=&gt;'35','offense_max'=&gt;'46.6','defense_inf'=&gt;'40','defense_inf_max'=&gt;'52.4','defense_cav'=&gt;'30','defense_cav_max'=&gt;'40.9','cost'=&gt;'290','cost_wood'=&gt;'130','cost_clay'=&gt;'80','cost_iron'=&gt;'40','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'h01'),</v>
       </c>
       <c r="W62" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h01','Hun',7,'Mercenary',3,1,30,6,35,46.6,40,52.4,30,40.9,290,130,80,40,40,0,'h01.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h01','Hun',7,'Mercenary',3,1,30,6,35,46.6,40,52.4,30,40.9,290,130,80,40,40,0,'h01','array('id'=&gt;'h01','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Mercenary','type'=&gt;'3','upkeep'=&gt;'1','carry'=&gt;'30','speed'=&gt;'6','offense'=&gt;'35','offense_max'=&gt;'46.6','defense_inf'=&gt;'40','defense_inf_max'=&gt;'52.4','defense_cav'=&gt;'30','defense_cav_max'=&gt;'40.9','cost'=&gt;'290','cost_wood'=&gt;'130','cost_clay'=&gt;'80','cost_iron'=&gt;'40','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'h01'),');</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.3">
@@ -5517,12 +5652,17 @@
       <c r="T63" s="3">
         <v>0</v>
       </c>
-      <c r="U63" t="s">
-        <v>222</v>
+      <c r="U63" t="str">
+        <f t="shared" si="0"/>
+        <v>h02</v>
+      </c>
+      <c r="V63" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'h02','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Bowman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'10','speed'=&gt;'6','offense'=&gt;'50','offense_max'=&gt;'63.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'40.9','defense_cav'=&gt;'10','defense_cav_max'=&gt;'17.9','cost'=&gt;'370','cost_wood'=&gt;'140','cost_clay'=&gt;'110','cost_iron'=&gt;'60','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'h02'),</v>
       </c>
       <c r="W63" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h02','Hun',7,'Bowman',2,1,10,6,50,63.9,30,40.9,10,17.9,370,140,110,60,60,0,'h02.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h02','Hun',7,'Bowman',2,1,10,6,50,63.9,30,40.9,10,17.9,370,140,110,60,60,0,'h02','array('id'=&gt;'h02','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Bowman','type'=&gt;'2','upkeep'=&gt;'1','carry'=&gt;'10','speed'=&gt;'6','offense'=&gt;'50','offense_max'=&gt;'63.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'40.9','defense_cav'=&gt;'10','defense_cav_max'=&gt;'17.9','cost'=&gt;'370','cost_wood'=&gt;'140','cost_clay'=&gt;'110','cost_iron'=&gt;'60','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'h02'),');</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.3">
@@ -5586,12 +5726,17 @@
       <c r="T64" s="3">
         <v>0</v>
       </c>
-      <c r="U64" t="s">
-        <v>223</v>
+      <c r="U64" t="str">
+        <f t="shared" si="0"/>
+        <v>h03</v>
+      </c>
+      <c r="V64" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'h03','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Spotter','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'10','speed'=&gt;'19','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'380','cost_wood'=&gt;'170','cost_clay'=&gt;'150','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'h03'),</v>
       </c>
       <c r="W64" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h03','Hun',7,'Spotter',0,2,10,19,0,12.7,20,35.7,10,24.2,380,170,150,20,40,0,'h03.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h03','Hun',7,'Spotter',0,2,10,19,0,12.7,20,35.7,10,24.2,380,170,150,20,40,0,'h03','array('id'=&gt;'h03','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Spotter','type'=&gt;'0','upkeep'=&gt;'2','carry'=&gt;'10','speed'=&gt;'19','offense'=&gt;'0','offense_max'=&gt;'12.7','defense_inf'=&gt;'20','defense_inf_max'=&gt;'35.7','defense_cav'=&gt;'10','defense_cav_max'=&gt;'24.2','cost'=&gt;'380','cost_wood'=&gt;'170','cost_clay'=&gt;'150','cost_iron'=&gt;'20','cost_crop'=&gt;'40','time'=&gt;'0','image'=&gt;'h03'),');</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.3">
@@ -5655,12 +5800,17 @@
       <c r="T65" s="3">
         <v>0</v>
       </c>
-      <c r="U65" t="s">
-        <v>224</v>
+      <c r="U65" t="str">
+        <f t="shared" si="0"/>
+        <v>h04</v>
+      </c>
+      <c r="V65" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'h04','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Steppe Rider','type'=&gt;'4','upkeep'=&gt;'2','carry'=&gt;'15','speed'=&gt;'16','offense'=&gt;'120','offense_max'=&gt;'150.7','defense_inf'=&gt;'30','defense_inf_max'=&gt;'47.2','defense_cav'=&gt;'15','defense_cav_max'=&gt;'30','cost'=&gt;'895','cost_wood'=&gt;'290','cost_clay'=&gt;'370','cost_iron'=&gt;'190','cost_crop'=&gt;'45','time'=&gt;'0','image'=&gt;'h04'),</v>
       </c>
       <c r="W65" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h04','Hun',7,'Steppe Rider',4,2,15,16,120,150.7,30,47.2,15,30,895,290,370,190,45,0,'h04.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h04','Hun',7,'Steppe Rider',4,2,15,16,120,150.7,30,47.2,15,30,895,290,370,190,45,0,'h04','array('id'=&gt;'h04','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Steppe Rider','type'=&gt;'4','upkeep'=&gt;'2','carry'=&gt;'15','speed'=&gt;'16','offense'=&gt;'120','offense_max'=&gt;'150.7','defense_inf'=&gt;'30','defense_inf_max'=&gt;'47.2','defense_cav'=&gt;'15','defense_cav_max'=&gt;'30','cost'=&gt;'895','cost_wood'=&gt;'290','cost_clay'=&gt;'370','cost_iron'=&gt;'190','cost_crop'=&gt;'45','time'=&gt;'0','image'=&gt;'h04'),');</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.3">
@@ -5724,12 +5874,17 @@
       <c r="T66" s="3">
         <v>0</v>
       </c>
-      <c r="U66" t="s">
-        <v>225</v>
+      <c r="U66" t="str">
+        <f t="shared" si="0"/>
+        <v>h05</v>
+      </c>
+      <c r="V66" t="str">
+        <f t="shared" si="1"/>
+        <v>array('id'=&gt;'h05','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Marksman','type'=&gt;'7','upkeep'=&gt;'2','carry'=&gt;'70','speed'=&gt;'16','offense'=&gt;'115','offense_max'=&gt;'145','defense_inf'=&gt;'80','defense_inf_max'=&gt;'104.7','defense_cav'=&gt;'70','defense_cav_max'=&gt;'93.2','cost'=&gt;'1050','cost_wood'=&gt;'320','cost_clay'=&gt;'350','cost_iron'=&gt;'330','cost_crop'=&gt;'50','time'=&gt;'0','image'=&gt;'h05'),</v>
       </c>
       <c r="W66" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h05','Hun',7,'Marksman',7,2,70,16,115,145,80,104.7,70,93.2,1050,320,350,330,50,0,'h05.png','');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h05','Hun',7,'Marksman',7,2,70,16,115,145,80,104.7,70,93.2,1050,320,350,330,50,0,'h05','array('id'=&gt;'h05','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Marksman','type'=&gt;'7','upkeep'=&gt;'2','carry'=&gt;'70','speed'=&gt;'16','offense'=&gt;'115','offense_max'=&gt;'145','defense_inf'=&gt;'80','defense_inf_max'=&gt;'104.7','defense_cav'=&gt;'70','defense_cav_max'=&gt;'93.2','cost'=&gt;'1050','cost_wood'=&gt;'320','cost_clay'=&gt;'350','cost_iron'=&gt;'330','cost_crop'=&gt;'50','time'=&gt;'0','image'=&gt;'h05'),');</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.3">
@@ -5793,12 +5948,17 @@
       <c r="T67" s="3">
         <v>0</v>
       </c>
-      <c r="U67" t="s">
-        <v>226</v>
+      <c r="U67" t="str">
+        <f t="shared" ref="U67:U71" si="3">A67</f>
+        <v>h06</v>
+      </c>
+      <c r="V67" t="str">
+        <f t="shared" ref="V67:V71" si="4">CONCATENATE("array('id'=&gt;'",A67,"','tribe'=&gt;'",B67,"','tribe_id'=&gt;'",C67,"','name'=&gt;'",D67,"','type'=&gt;'",E67,"','upkeep'=&gt;'",F67,"','carry'=&gt;'",G67,"','speed'=&gt;'",H67,"','offense'=&gt;'",I67,"','offense_max'=&gt;'",J67,"','defense_inf'=&gt;'",K67,"','defense_inf_max'=&gt;'",L67,"','defense_cav'=&gt;'",M67,"','defense_cav_max'=&gt;'",N67,"','cost'=&gt;'",O67,"','cost_wood'=&gt;'",P67,"','cost_clay'=&gt;'",Q67,"','cost_iron'=&gt;'",R67,"','cost_crop'=&gt;'",S67,"','time'=&gt;'",T67,"','image'=&gt;'",U67,"'),")</f>
+        <v>array('id'=&gt;'h06','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Marauder','type'=&gt;'4','upkeep'=&gt;'3','carry'=&gt;'40','speed'=&gt;'14','offense'=&gt;'180','offense_max'=&gt;'226.1','defense_inf'=&gt;'60','defense_inf_max'=&gt;'88.1','defense_cav'=&gt;'40','defense_cav_max'=&gt;'65.1','cost'=&gt;'1760','cost_wood'=&gt;'450','cost_clay'=&gt;'560','cost_iron'=&gt;'610','cost_crop'=&gt;'140','time'=&gt;'0','image'=&gt;'h06'),</v>
       </c>
       <c r="W67" t="str">
-        <f t="shared" ref="W67:W71" si="1">CONCATENATE("INSERT INTO UNITS_DETAILS VALUES ('",A67,"','",B67,"',",C67,",'",D67,"',",E67,",",F67,",",G67,",",H67,",",I67,",",J67,",",K67,",",L67,",",M67,",",N67,",",O67,",",P67,",",Q67,",",R67,",",S67,",",T67,",'",U67,"','",V67,"');")</f>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h06','Hun',7,'Marauder',4,3,40,14,180,226.1,60,88.1,40,65.1,1760,450,560,610,140,0,'h06.png','');</v>
+        <f t="shared" ref="W67:W71" si="5">CONCATENATE("INSERT INTO UNITS_DETAILS VALUES ('",A67,"','",B67,"',",C67,",'",D67,"',",E67,",",F67,",",G67,",",H67,",",I67,",",J67,",",K67,",",L67,",",M67,",",N67,",",O67,",",P67,",",Q67,",",R67,",",S67,",",T67,",'",U67,"','",V67,"');")</f>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h06','Hun',7,'Marauder',4,3,40,14,180,226.1,60,88.1,40,65.1,1760,450,560,610,140,0,'h06','array('id'=&gt;'h06','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Marauder','type'=&gt;'4','upkeep'=&gt;'3','carry'=&gt;'40','speed'=&gt;'14','offense'=&gt;'180','offense_max'=&gt;'226.1','defense_inf'=&gt;'60','defense_inf_max'=&gt;'88.1','defense_cav'=&gt;'40','defense_cav_max'=&gt;'65.1','cost'=&gt;'1760','cost_wood'=&gt;'450','cost_clay'=&gt;'560','cost_iron'=&gt;'610','cost_crop'=&gt;'140','time'=&gt;'0','image'=&gt;'h06'),');</v>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.3">
@@ -5862,12 +6022,17 @@
       <c r="T68" s="3">
         <v>0</v>
       </c>
-      <c r="U68" t="s">
-        <v>227</v>
+      <c r="U68" t="str">
+        <f t="shared" si="3"/>
+        <v>h07</v>
+      </c>
+      <c r="V68" t="str">
+        <f t="shared" si="4"/>
+        <v>array('id'=&gt;'h07','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'90','speed'=&gt;'4','offense'=&gt;'65','offense_max'=&gt;'93.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'90','defense_cav_max'=&gt;'122.6','cost'=&gt;'1820','cost_wood'=&gt;'1060','cost_clay'=&gt;'330','cost_iron'=&gt;'360','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'h07'),</v>
       </c>
       <c r="W68" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h07','Hun',7,'Ram',6,3,90,4,65,93.9,30,53.6,90,122.6,1820,1060,330,360,70,0,'h07.png','');</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h07','Hun',7,'Ram',6,3,90,4,65,93.9,30,53.6,90,122.6,1820,1060,330,360,70,0,'h07','array('id'=&gt;'h07','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Ram','type'=&gt;'6','upkeep'=&gt;'3','carry'=&gt;'90','speed'=&gt;'4','offense'=&gt;'65','offense_max'=&gt;'93.9','defense_inf'=&gt;'30','defense_inf_max'=&gt;'53.6','defense_cav'=&gt;'90','defense_cav_max'=&gt;'122.6','cost'=&gt;'1820','cost_wood'=&gt;'1060','cost_clay'=&gt;'330','cost_iron'=&gt;'360','cost_crop'=&gt;'70','time'=&gt;'0','image'=&gt;'h07'),');</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.3">
@@ -5931,12 +6096,17 @@
       <c r="T69" s="3">
         <v>0</v>
       </c>
-      <c r="U69" t="s">
-        <v>228</v>
+      <c r="U69" t="str">
+        <f t="shared" si="3"/>
+        <v>h08</v>
+      </c>
+      <c r="V69" t="str">
+        <f t="shared" si="4"/>
+        <v>array('id'=&gt;'h08','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'10','speed'=&gt;'3','offense'=&gt;'45','offense_max'=&gt;'90','defense_inf'=&gt;'55','defense_inf_max'=&gt;'101.5','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'2910','cost_wood'=&gt;'950','cost_clay'=&gt;'1280','cost_iron'=&gt;'620','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'h08'),</v>
       </c>
       <c r="W69" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h08','Hun',7,'Catapult',6,6,10,3,45,90,55,101.5,10,49.7,2910,950,1280,620,60,0,'h08.png','');</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h08','Hun',7,'Catapult',6,6,10,3,45,90,55,101.5,10,49.7,2910,950,1280,620,60,0,'h08','array('id'=&gt;'h08','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Catapult','type'=&gt;'6','upkeep'=&gt;'6','carry'=&gt;'10','speed'=&gt;'3','offense'=&gt;'45','offense_max'=&gt;'90','defense_inf'=&gt;'55','defense_inf_max'=&gt;'101.5','defense_cav'=&gt;'10','defense_cav_max'=&gt;'49.7','cost'=&gt;'2910','cost_wood'=&gt;'950','cost_clay'=&gt;'1280','cost_iron'=&gt;'620','cost_crop'=&gt;'60','time'=&gt;'0','image'=&gt;'h08'),');</v>
       </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.3">
@@ -6000,12 +6170,17 @@
       <c r="T70" s="3">
         <v>0</v>
       </c>
-      <c r="U70" t="s">
-        <v>229</v>
+      <c r="U70" t="str">
+        <f t="shared" si="3"/>
+        <v>h09</v>
+      </c>
+      <c r="V70" t="str">
+        <f t="shared" si="4"/>
+        <v>array('id'=&gt;'h09','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Logades','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'50','speed'=&gt;'5','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'117600','cost_wood'=&gt;'37200','cost_clay'=&gt;'27600','cost_iron'=&gt;'25200','cost_crop'=&gt;'27600','time'=&gt;'0','image'=&gt;'h09'),</v>
       </c>
       <c r="W70" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h09','Hun',7,'Logades',8,4,50,5,40,40,50,50,50,50,117600,37200,27600,25200,27600,0,'h09.png','');</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h09','Hun',7,'Logades',8,4,50,5,40,40,50,50,50,50,117600,37200,27600,25200,27600,0,'h09','array('id'=&gt;'h09','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Logades','type'=&gt;'8','upkeep'=&gt;'4','carry'=&gt;'50','speed'=&gt;'5','offense'=&gt;'40','offense_max'=&gt;'40','defense_inf'=&gt;'50','defense_inf_max'=&gt;'50','defense_cav'=&gt;'50','defense_cav_max'=&gt;'50','cost'=&gt;'117600','cost_wood'=&gt;'37200','cost_clay'=&gt;'27600','cost_iron'=&gt;'25200','cost_crop'=&gt;'27600','time'=&gt;'0','image'=&gt;'h09'),');</v>
       </c>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.3">
@@ -6069,12 +6244,17 @@
       <c r="T71" s="3">
         <v>0</v>
       </c>
-      <c r="U71" t="s">
-        <v>230</v>
+      <c r="U71" t="str">
+        <f t="shared" si="3"/>
+        <v>h10</v>
+      </c>
+      <c r="V71" t="str">
+        <f t="shared" si="4"/>
+        <v>array('id'=&gt;'h10','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'80','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'20900','cost_wood'=&gt;'6100','cost_clay'=&gt;'4600','cost_iron'=&gt;'4800','cost_crop'=&gt;'5400','time'=&gt;'0','image'=&gt;'h10'),</v>
       </c>
       <c r="W71" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO UNITS_DETAILS VALUES ('h10','Hun',7,'Settler',8,1,80,5,0,0,80,80,80,80,20900,6100,4600,4800,5400,0,'h10.png','');</v>
+        <f t="shared" si="5"/>
+        <v>INSERT INTO UNITS_DETAILS VALUES ('h10','Hun',7,'Settler',8,1,80,5,0,0,80,80,80,80,20900,6100,4600,4800,5400,0,'h10','array('id'=&gt;'h10','tribe'=&gt;'Hun','tribe_id'=&gt;'7','name'=&gt;'Settler','type'=&gt;'8','upkeep'=&gt;'1','carry'=&gt;'80','speed'=&gt;'5','offense'=&gt;'0','offense_max'=&gt;'0','defense_inf'=&gt;'80','defense_inf_max'=&gt;'80','defense_cav'=&gt;'80','defense_cav_max'=&gt;'80','cost'=&gt;'20900','cost_wood'=&gt;'6100','cost_clay'=&gt;'4600','cost_iron'=&gt;'4800','cost_crop'=&gt;'5400','time'=&gt;'0','image'=&gt;'h10'),');</v>
       </c>
     </row>
   </sheetData>
@@ -6084,7 +6264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Incomings Controller update and Leader incomings added
</commit_message>
<xml_diff>
--- a/Scripts/sql/units_metaData.xlsx
+++ b/Scripts/sql/units_metaData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1CEDEB-28AA-4E8E-9C1A-4964ECD70128}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AEE4A7-751D-4EE2-AD46-55DA019822D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -998,10 +998,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>